<commit_message>
Changes to tune results
</commit_message>
<xml_diff>
--- a/HealthPath/CreatingReport/Matrix.xlsx
+++ b/HealthPath/CreatingReport/Matrix.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="773" uniqueCount="536">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="776" uniqueCount="536">
   <si>
     <t xml:space="preserve">Code</t>
   </si>
@@ -1348,6 +1348,12 @@
     <t xml:space="preserve">Escherichia coli (E. coli) is a species of gram-negative bacteria. It’s a normal part of the gut microbiome, and most strains don’t cause problems in humans.</t>
   </si>
   <si>
+    <t xml:space="preserve">1,0 x 10^4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">9,0 x 10^4</t>
+  </si>
+  <si>
     <t xml:space="preserve">10^6 : 9,9x10^6</t>
   </si>
   <si>
@@ -1373,12 +1379,6 @@
   </si>
   <si>
     <t xml:space="preserve">These species of bacteria are a normal part of a gut microbiome, and most don’t cause problems in humans.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1,0 x 10^4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">9,0 x 10^4</t>
   </si>
   <si>
     <t xml:space="preserve">10^6 : 9,9x10^7</t>
@@ -2254,6 +2254,7 @@
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -2487,7 +2488,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="120">
+  <cellXfs count="121">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -2824,6 +2825,10 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="165" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -3047,8 +3052,8 @@
   </sheetPr>
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D107" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G133" activeCellId="0" sqref="G133"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D174" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F194" activeCellId="0" sqref="F194"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -6736,20 +6741,26 @@
       <c r="D187" s="37" t="s">
         <v>329</v>
       </c>
-      <c r="E187" s="17"/>
-      <c r="F187" s="17"/>
-      <c r="G187" s="17"/>
-      <c r="H187" s="17" t="s">
+      <c r="E187" s="84" t="s">
+        <v>249</v>
+      </c>
+      <c r="F187" s="84" t="s">
         <v>330</v>
       </c>
-      <c r="I187" s="17" t="s">
+      <c r="G187" s="84" t="s">
         <v>331</v>
       </c>
-      <c r="J187" s="17" t="s">
+      <c r="H187" s="84" t="s">
         <v>332</v>
       </c>
-      <c r="K187" s="17" t="s">
+      <c r="I187" s="84" t="s">
         <v>333</v>
+      </c>
+      <c r="J187" s="84" t="s">
+        <v>334</v>
+      </c>
+      <c r="K187" s="84" t="s">
+        <v>335</v>
       </c>
       <c r="L187" s="17"/>
       <c r="M187" s="12"/>
@@ -6763,20 +6774,20 @@
       <c r="E188" s="17"/>
       <c r="F188" s="17"/>
       <c r="G188" s="17"/>
-      <c r="H188" s="84"/>
-      <c r="I188" s="84"/>
-      <c r="J188" s="84"/>
-      <c r="K188" s="84"/>
+      <c r="H188" s="85"/>
+      <c r="I188" s="85"/>
+      <c r="J188" s="85"/>
+      <c r="K188" s="85"/>
       <c r="L188" s="17"/>
       <c r="M188" s="12"/>
     </row>
     <row r="189" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B189" s="53"/>
       <c r="C189" s="60" t="s">
-        <v>334</v>
+        <v>336</v>
       </c>
       <c r="D189" s="79" t="s">
-        <v>335</v>
+        <v>337</v>
       </c>
       <c r="E189" s="17"/>
       <c r="F189" s="17"/>
@@ -6818,40 +6829,40 @@
     </row>
     <row r="192" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A192" s="13" t="s">
-        <v>336</v>
+        <v>338</v>
       </c>
       <c r="B192" s="27" t="s">
-        <v>337</v>
+        <v>339</v>
       </c>
       <c r="C192" s="36" t="s">
-        <v>338</v>
+        <v>340</v>
       </c>
       <c r="D192" s="37" t="s">
-        <v>338</v>
+        <v>340</v>
       </c>
       <c r="E192" s="25" t="s">
         <v>249</v>
       </c>
       <c r="F192" s="17" t="s">
-        <v>339</v>
+        <v>330</v>
       </c>
       <c r="G192" s="17" t="s">
-        <v>340</v>
+        <v>331</v>
       </c>
       <c r="H192" s="17" t="s">
         <v>341</v>
       </c>
       <c r="I192" s="17" t="s">
-        <v>331</v>
+        <v>333</v>
       </c>
       <c r="J192" s="17" t="s">
-        <v>332</v>
+        <v>334</v>
       </c>
       <c r="K192" s="17" t="s">
-        <v>333</v>
+        <v>335</v>
       </c>
       <c r="L192" s="17"/>
-      <c r="M192" s="85"/>
+      <c r="M192" s="86"/>
     </row>
     <row r="193" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B193" s="30" t="s">
@@ -6902,7 +6913,7 @@
       <c r="M195" s="12"/>
     </row>
     <row r="196" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A196" s="86" t="s">
+      <c r="A196" s="87" t="s">
         <v>344</v>
       </c>
       <c r="B196" s="27" t="s">
@@ -6918,7 +6929,7 @@
         <v>249</v>
       </c>
       <c r="F196" s="17" t="s">
-        <v>339</v>
+        <v>330</v>
       </c>
       <c r="G196" s="17" t="s">
         <v>347</v>
@@ -7001,7 +7012,7 @@
       <c r="M200" s="12"/>
     </row>
     <row r="201" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A201" s="86" t="s">
+      <c r="A201" s="87" t="s">
         <v>354</v>
       </c>
       <c r="B201" s="27" t="s">
@@ -7189,7 +7200,7 @@
         <v>367</v>
       </c>
       <c r="I210" s="17" t="s">
-        <v>339</v>
+        <v>330</v>
       </c>
       <c r="J210" s="17" t="s">
         <v>250</v>
@@ -7278,7 +7289,7 @@
         <v>367</v>
       </c>
       <c r="I215" s="17" t="s">
-        <v>339</v>
+        <v>330</v>
       </c>
       <c r="J215" s="17" t="s">
         <v>250</v>
@@ -7339,7 +7350,7 @@
         <v>367</v>
       </c>
       <c r="I218" s="17" t="s">
-        <v>339</v>
+        <v>330</v>
       </c>
       <c r="J218" s="17" t="s">
         <v>250</v>
@@ -7389,7 +7400,7 @@
       <c r="B221" s="27" t="s">
         <v>380</v>
       </c>
-      <c r="C221" s="87" t="s">
+      <c r="C221" s="88" t="s">
         <v>381</v>
       </c>
       <c r="D221" s="55"/>
@@ -7411,7 +7422,7 @@
       <c r="B222" s="42" t="s">
         <v>382</v>
       </c>
-      <c r="C222" s="87"/>
+      <c r="C222" s="88"/>
       <c r="D222" s="55"/>
       <c r="E222" s="17"/>
       <c r="F222" s="17"/>
@@ -7577,7 +7588,7 @@
       <c r="A231" s="26" t="s">
         <v>396</v>
       </c>
-      <c r="B231" s="88" t="s">
+      <c r="B231" s="89" t="s">
         <v>397</v>
       </c>
       <c r="C231" s="80" t="s">
@@ -7873,7 +7884,7 @@
     </row>
     <row r="246" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B246" s="31"/>
-      <c r="C246" s="89" t="s">
+      <c r="C246" s="90" t="s">
         <v>421</v>
       </c>
       <c r="D246" s="55"/>
@@ -7888,11 +7899,11 @@
       <c r="M246" s="12"/>
     </row>
     <row r="247" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B247" s="90" t="s">
+      <c r="B247" s="91" t="s">
         <v>422</v>
       </c>
-      <c r="C247" s="90"/>
-      <c r="D247" s="90"/>
+      <c r="C247" s="91"/>
+      <c r="D247" s="91"/>
       <c r="E247" s="17"/>
       <c r="F247" s="17"/>
       <c r="G247" s="17"/>
@@ -7904,16 +7915,16 @@
       <c r="M247" s="12"/>
     </row>
     <row r="248" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A248" s="91" t="s">
+      <c r="A248" s="92" t="s">
         <v>423</v>
       </c>
-      <c r="B248" s="92" t="s">
+      <c r="B248" s="93" t="s">
         <v>424</v>
       </c>
-      <c r="C248" s="93" t="s">
+      <c r="C248" s="94" t="s">
         <v>425</v>
       </c>
-      <c r="D248" s="94"/>
+      <c r="D248" s="95"/>
       <c r="E248" s="25"/>
       <c r="F248" s="25"/>
       <c r="G248" s="25"/>
@@ -7922,28 +7933,28 @@
       <c r="J248" s="25"/>
       <c r="K248" s="25"/>
       <c r="L248" s="25"/>
-      <c r="M248" s="95"/>
-      <c r="N248" s="91"/>
-      <c r="O248" s="91"/>
-      <c r="P248" s="91"/>
-      <c r="Q248" s="91"/>
-      <c r="R248" s="91"/>
-      <c r="S248" s="91"/>
-      <c r="T248" s="91"/>
-      <c r="U248" s="91"/>
-      <c r="V248" s="91"/>
-      <c r="W248" s="91"/>
-      <c r="X248" s="91"/>
-      <c r="Y248" s="91"/>
-      <c r="Z248" s="91"/>
+      <c r="M248" s="96"/>
+      <c r="N248" s="92"/>
+      <c r="O248" s="92"/>
+      <c r="P248" s="92"/>
+      <c r="Q248" s="92"/>
+      <c r="R248" s="92"/>
+      <c r="S248" s="92"/>
+      <c r="T248" s="92"/>
+      <c r="U248" s="92"/>
+      <c r="V248" s="92"/>
+      <c r="W248" s="92"/>
+      <c r="X248" s="92"/>
+      <c r="Y248" s="92"/>
+      <c r="Z248" s="92"/>
     </row>
     <row r="249" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A249" s="91"/>
-      <c r="B249" s="96" t="s">
+      <c r="A249" s="92"/>
+      <c r="B249" s="97" t="s">
         <v>426</v>
       </c>
-      <c r="C249" s="93"/>
-      <c r="D249" s="94"/>
+      <c r="C249" s="94"/>
+      <c r="D249" s="95"/>
       <c r="E249" s="25"/>
       <c r="F249" s="25"/>
       <c r="G249" s="25"/>
@@ -7952,28 +7963,28 @@
       <c r="J249" s="25"/>
       <c r="K249" s="25"/>
       <c r="L249" s="25"/>
-      <c r="M249" s="95"/>
-      <c r="N249" s="91"/>
-      <c r="O249" s="91"/>
-      <c r="P249" s="91"/>
-      <c r="Q249" s="91"/>
-      <c r="R249" s="91"/>
-      <c r="S249" s="91"/>
-      <c r="T249" s="91"/>
-      <c r="U249" s="91"/>
-      <c r="V249" s="91"/>
-      <c r="W249" s="91"/>
-      <c r="X249" s="91"/>
-      <c r="Y249" s="91"/>
-      <c r="Z249" s="91"/>
+      <c r="M249" s="96"/>
+      <c r="N249" s="92"/>
+      <c r="O249" s="92"/>
+      <c r="P249" s="92"/>
+      <c r="Q249" s="92"/>
+      <c r="R249" s="92"/>
+      <c r="S249" s="92"/>
+      <c r="T249" s="92"/>
+      <c r="U249" s="92"/>
+      <c r="V249" s="92"/>
+      <c r="W249" s="92"/>
+      <c r="X249" s="92"/>
+      <c r="Y249" s="92"/>
+      <c r="Z249" s="92"/>
     </row>
     <row r="250" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A250" s="91"/>
-      <c r="B250" s="97"/>
-      <c r="C250" s="93" t="s">
+      <c r="A250" s="92"/>
+      <c r="B250" s="98"/>
+      <c r="C250" s="94" t="s">
         <v>427</v>
       </c>
-      <c r="D250" s="94"/>
+      <c r="D250" s="95"/>
       <c r="E250" s="25"/>
       <c r="F250" s="25"/>
       <c r="G250" s="25"/>
@@ -7982,28 +7993,28 @@
       <c r="J250" s="25"/>
       <c r="K250" s="25"/>
       <c r="L250" s="25"/>
-      <c r="M250" s="95"/>
-      <c r="N250" s="91"/>
-      <c r="O250" s="91"/>
-      <c r="P250" s="91"/>
-      <c r="Q250" s="91"/>
-      <c r="R250" s="91"/>
-      <c r="S250" s="91"/>
-      <c r="T250" s="91"/>
-      <c r="U250" s="91"/>
-      <c r="V250" s="91"/>
-      <c r="W250" s="91"/>
-      <c r="X250" s="91"/>
-      <c r="Y250" s="91"/>
-      <c r="Z250" s="91"/>
+      <c r="M250" s="96"/>
+      <c r="N250" s="92"/>
+      <c r="O250" s="92"/>
+      <c r="P250" s="92"/>
+      <c r="Q250" s="92"/>
+      <c r="R250" s="92"/>
+      <c r="S250" s="92"/>
+      <c r="T250" s="92"/>
+      <c r="U250" s="92"/>
+      <c r="V250" s="92"/>
+      <c r="W250" s="92"/>
+      <c r="X250" s="92"/>
+      <c r="Y250" s="92"/>
+      <c r="Z250" s="92"/>
     </row>
     <row r="251" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A251" s="91"/>
-      <c r="B251" s="98" t="s">
+      <c r="A251" s="92"/>
+      <c r="B251" s="99" t="s">
         <v>428</v>
       </c>
-      <c r="C251" s="93"/>
-      <c r="D251" s="94"/>
+      <c r="C251" s="94"/>
+      <c r="D251" s="95"/>
       <c r="E251" s="25"/>
       <c r="F251" s="25"/>
       <c r="G251" s="25"/>
@@ -8012,30 +8023,30 @@
       <c r="J251" s="25"/>
       <c r="K251" s="25"/>
       <c r="L251" s="25"/>
-      <c r="M251" s="95"/>
-      <c r="N251" s="91"/>
-      <c r="O251" s="91"/>
-      <c r="P251" s="91"/>
-      <c r="Q251" s="91"/>
-      <c r="R251" s="91"/>
-      <c r="S251" s="91"/>
-      <c r="T251" s="91"/>
-      <c r="U251" s="91"/>
-      <c r="V251" s="91"/>
-      <c r="W251" s="91"/>
-      <c r="X251" s="91"/>
-      <c r="Y251" s="91"/>
-      <c r="Z251" s="91"/>
+      <c r="M251" s="96"/>
+      <c r="N251" s="92"/>
+      <c r="O251" s="92"/>
+      <c r="P251" s="92"/>
+      <c r="Q251" s="92"/>
+      <c r="R251" s="92"/>
+      <c r="S251" s="92"/>
+      <c r="T251" s="92"/>
+      <c r="U251" s="92"/>
+      <c r="V251" s="92"/>
+      <c r="W251" s="92"/>
+      <c r="X251" s="92"/>
+      <c r="Y251" s="92"/>
+      <c r="Z251" s="92"/>
     </row>
     <row r="252" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A252" s="91"/>
-      <c r="B252" s="98" t="s">
+      <c r="A252" s="92"/>
+      <c r="B252" s="99" t="s">
         <v>429</v>
       </c>
-      <c r="C252" s="99" t="s">
+      <c r="C252" s="100" t="s">
         <v>430</v>
       </c>
-      <c r="D252" s="94"/>
+      <c r="D252" s="95"/>
       <c r="E252" s="25"/>
       <c r="F252" s="25"/>
       <c r="G252" s="25"/>
@@ -8044,30 +8055,30 @@
       <c r="J252" s="25"/>
       <c r="K252" s="25"/>
       <c r="L252" s="25"/>
-      <c r="M252" s="95"/>
-      <c r="N252" s="91"/>
-      <c r="O252" s="91"/>
-      <c r="P252" s="91"/>
-      <c r="Q252" s="91"/>
-      <c r="R252" s="91"/>
-      <c r="S252" s="91"/>
-      <c r="T252" s="91"/>
-      <c r="U252" s="91"/>
-      <c r="V252" s="91"/>
-      <c r="W252" s="91"/>
-      <c r="X252" s="91"/>
-      <c r="Y252" s="91"/>
-      <c r="Z252" s="91"/>
+      <c r="M252" s="96"/>
+      <c r="N252" s="92"/>
+      <c r="O252" s="92"/>
+      <c r="P252" s="92"/>
+      <c r="Q252" s="92"/>
+      <c r="R252" s="92"/>
+      <c r="S252" s="92"/>
+      <c r="T252" s="92"/>
+      <c r="U252" s="92"/>
+      <c r="V252" s="92"/>
+      <c r="W252" s="92"/>
+      <c r="X252" s="92"/>
+      <c r="Y252" s="92"/>
+      <c r="Z252" s="92"/>
     </row>
     <row r="253" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A253" s="91"/>
-      <c r="B253" s="92" t="s">
+      <c r="A253" s="92"/>
+      <c r="B253" s="93" t="s">
         <v>431</v>
       </c>
-      <c r="C253" s="93" t="s">
+      <c r="C253" s="94" t="s">
         <v>432</v>
       </c>
-      <c r="D253" s="94"/>
+      <c r="D253" s="95"/>
       <c r="E253" s="25"/>
       <c r="F253" s="25"/>
       <c r="G253" s="25"/>
@@ -8080,28 +8091,28 @@
       </c>
       <c r="K253" s="25"/>
       <c r="L253" s="25"/>
-      <c r="M253" s="95"/>
-      <c r="N253" s="91"/>
-      <c r="O253" s="91"/>
-      <c r="P253" s="91"/>
-      <c r="Q253" s="91"/>
-      <c r="R253" s="91"/>
-      <c r="S253" s="91"/>
-      <c r="T253" s="91"/>
-      <c r="U253" s="91"/>
-      <c r="V253" s="91"/>
-      <c r="W253" s="91"/>
-      <c r="X253" s="91"/>
-      <c r="Y253" s="91"/>
-      <c r="Z253" s="91"/>
+      <c r="M253" s="96"/>
+      <c r="N253" s="92"/>
+      <c r="O253" s="92"/>
+      <c r="P253" s="92"/>
+      <c r="Q253" s="92"/>
+      <c r="R253" s="92"/>
+      <c r="S253" s="92"/>
+      <c r="T253" s="92"/>
+      <c r="U253" s="92"/>
+      <c r="V253" s="92"/>
+      <c r="W253" s="92"/>
+      <c r="X253" s="92"/>
+      <c r="Y253" s="92"/>
+      <c r="Z253" s="92"/>
     </row>
     <row r="254" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A254" s="91"/>
-      <c r="B254" s="96" t="s">
+      <c r="A254" s="92"/>
+      <c r="B254" s="97" t="s">
         <v>433</v>
       </c>
-      <c r="C254" s="93"/>
-      <c r="D254" s="94"/>
+      <c r="C254" s="94"/>
+      <c r="D254" s="95"/>
       <c r="E254" s="25"/>
       <c r="F254" s="25"/>
       <c r="G254" s="25"/>
@@ -8110,28 +8121,28 @@
       <c r="J254" s="25"/>
       <c r="K254" s="25"/>
       <c r="L254" s="25"/>
-      <c r="M254" s="95"/>
-      <c r="N254" s="91"/>
-      <c r="O254" s="91"/>
-      <c r="P254" s="91"/>
-      <c r="Q254" s="91"/>
-      <c r="R254" s="91"/>
-      <c r="S254" s="91"/>
-      <c r="T254" s="91"/>
-      <c r="U254" s="91"/>
-      <c r="V254" s="91"/>
-      <c r="W254" s="91"/>
-      <c r="X254" s="91"/>
-      <c r="Y254" s="91"/>
-      <c r="Z254" s="91"/>
+      <c r="M254" s="96"/>
+      <c r="N254" s="92"/>
+      <c r="O254" s="92"/>
+      <c r="P254" s="92"/>
+      <c r="Q254" s="92"/>
+      <c r="R254" s="92"/>
+      <c r="S254" s="92"/>
+      <c r="T254" s="92"/>
+      <c r="U254" s="92"/>
+      <c r="V254" s="92"/>
+      <c r="W254" s="92"/>
+      <c r="X254" s="92"/>
+      <c r="Y254" s="92"/>
+      <c r="Z254" s="92"/>
     </row>
     <row r="255" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A255" s="91"/>
-      <c r="B255" s="97"/>
-      <c r="C255" s="99" t="s">
+      <c r="A255" s="92"/>
+      <c r="B255" s="98"/>
+      <c r="C255" s="100" t="s">
         <v>434</v>
       </c>
-      <c r="D255" s="94"/>
+      <c r="D255" s="95"/>
       <c r="E255" s="25"/>
       <c r="F255" s="25"/>
       <c r="G255" s="25"/>
@@ -8144,30 +8155,30 @@
       </c>
       <c r="K255" s="25"/>
       <c r="L255" s="25"/>
-      <c r="M255" s="95"/>
-      <c r="N255" s="91"/>
-      <c r="O255" s="91"/>
-      <c r="P255" s="91"/>
-      <c r="Q255" s="91"/>
-      <c r="R255" s="91"/>
-      <c r="S255" s="91"/>
-      <c r="T255" s="91"/>
-      <c r="U255" s="91"/>
-      <c r="V255" s="91"/>
-      <c r="W255" s="91"/>
-      <c r="X255" s="91"/>
-      <c r="Y255" s="91"/>
-      <c r="Z255" s="91"/>
+      <c r="M255" s="96"/>
+      <c r="N255" s="92"/>
+      <c r="O255" s="92"/>
+      <c r="P255" s="92"/>
+      <c r="Q255" s="92"/>
+      <c r="R255" s="92"/>
+      <c r="S255" s="92"/>
+      <c r="T255" s="92"/>
+      <c r="U255" s="92"/>
+      <c r="V255" s="92"/>
+      <c r="W255" s="92"/>
+      <c r="X255" s="92"/>
+      <c r="Y255" s="92"/>
+      <c r="Z255" s="92"/>
     </row>
     <row r="256" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A256" s="91"/>
-      <c r="B256" s="92" t="s">
+      <c r="A256" s="92"/>
+      <c r="B256" s="93" t="s">
         <v>435</v>
       </c>
-      <c r="C256" s="93" t="s">
+      <c r="C256" s="94" t="s">
         <v>436</v>
       </c>
-      <c r="D256" s="94"/>
+      <c r="D256" s="95"/>
       <c r="E256" s="25"/>
       <c r="F256" s="25"/>
       <c r="G256" s="25"/>
@@ -8176,28 +8187,28 @@
       <c r="J256" s="25"/>
       <c r="K256" s="25"/>
       <c r="L256" s="25"/>
-      <c r="M256" s="95"/>
-      <c r="N256" s="91"/>
-      <c r="O256" s="91"/>
-      <c r="P256" s="91"/>
-      <c r="Q256" s="91"/>
-      <c r="R256" s="91"/>
-      <c r="S256" s="91"/>
-      <c r="T256" s="91"/>
-      <c r="U256" s="91"/>
-      <c r="V256" s="91"/>
-      <c r="W256" s="91"/>
-      <c r="X256" s="91"/>
-      <c r="Y256" s="91"/>
-      <c r="Z256" s="91"/>
+      <c r="M256" s="96"/>
+      <c r="N256" s="92"/>
+      <c r="O256" s="92"/>
+      <c r="P256" s="92"/>
+      <c r="Q256" s="92"/>
+      <c r="R256" s="92"/>
+      <c r="S256" s="92"/>
+      <c r="T256" s="92"/>
+      <c r="U256" s="92"/>
+      <c r="V256" s="92"/>
+      <c r="W256" s="92"/>
+      <c r="X256" s="92"/>
+      <c r="Y256" s="92"/>
+      <c r="Z256" s="92"/>
     </row>
     <row r="257" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A257" s="91"/>
-      <c r="B257" s="96" t="s">
+      <c r="A257" s="92"/>
+      <c r="B257" s="97" t="s">
         <v>437</v>
       </c>
-      <c r="C257" s="93"/>
-      <c r="D257" s="94"/>
+      <c r="C257" s="94"/>
+      <c r="D257" s="95"/>
       <c r="E257" s="25"/>
       <c r="F257" s="25"/>
       <c r="G257" s="25"/>
@@ -8206,28 +8217,28 @@
       <c r="J257" s="25"/>
       <c r="K257" s="25"/>
       <c r="L257" s="25"/>
-      <c r="M257" s="95"/>
-      <c r="N257" s="91"/>
-      <c r="O257" s="91"/>
-      <c r="P257" s="91"/>
-      <c r="Q257" s="91"/>
-      <c r="R257" s="91"/>
-      <c r="S257" s="91"/>
-      <c r="T257" s="91"/>
-      <c r="U257" s="91"/>
-      <c r="V257" s="91"/>
-      <c r="W257" s="91"/>
-      <c r="X257" s="91"/>
-      <c r="Y257" s="91"/>
-      <c r="Z257" s="91"/>
+      <c r="M257" s="96"/>
+      <c r="N257" s="92"/>
+      <c r="O257" s="92"/>
+      <c r="P257" s="92"/>
+      <c r="Q257" s="92"/>
+      <c r="R257" s="92"/>
+      <c r="S257" s="92"/>
+      <c r="T257" s="92"/>
+      <c r="U257" s="92"/>
+      <c r="V257" s="92"/>
+      <c r="W257" s="92"/>
+      <c r="X257" s="92"/>
+      <c r="Y257" s="92"/>
+      <c r="Z257" s="92"/>
     </row>
     <row r="258" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A258" s="91"/>
-      <c r="B258" s="97"/>
-      <c r="C258" s="99" t="s">
+      <c r="A258" s="92"/>
+      <c r="B258" s="98"/>
+      <c r="C258" s="100" t="s">
         <v>438</v>
       </c>
-      <c r="D258" s="94"/>
+      <c r="D258" s="95"/>
       <c r="E258" s="25"/>
       <c r="F258" s="25"/>
       <c r="G258" s="25"/>
@@ -8240,30 +8251,30 @@
       </c>
       <c r="K258" s="25"/>
       <c r="L258" s="25"/>
-      <c r="M258" s="95"/>
-      <c r="N258" s="91"/>
-      <c r="O258" s="91"/>
-      <c r="P258" s="91"/>
-      <c r="Q258" s="91"/>
-      <c r="R258" s="91"/>
-      <c r="S258" s="91"/>
-      <c r="T258" s="91"/>
-      <c r="U258" s="91"/>
-      <c r="V258" s="91"/>
-      <c r="W258" s="91"/>
-      <c r="X258" s="91"/>
-      <c r="Y258" s="91"/>
-      <c r="Z258" s="91"/>
+      <c r="M258" s="96"/>
+      <c r="N258" s="92"/>
+      <c r="O258" s="92"/>
+      <c r="P258" s="92"/>
+      <c r="Q258" s="92"/>
+      <c r="R258" s="92"/>
+      <c r="S258" s="92"/>
+      <c r="T258" s="92"/>
+      <c r="U258" s="92"/>
+      <c r="V258" s="92"/>
+      <c r="W258" s="92"/>
+      <c r="X258" s="92"/>
+      <c r="Y258" s="92"/>
+      <c r="Z258" s="92"/>
     </row>
     <row r="259" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A259" s="91"/>
-      <c r="B259" s="92" t="s">
+      <c r="A259" s="92"/>
+      <c r="B259" s="93" t="s">
         <v>439</v>
       </c>
-      <c r="C259" s="93" t="s">
+      <c r="C259" s="94" t="s">
         <v>440</v>
       </c>
-      <c r="D259" s="94"/>
+      <c r="D259" s="95"/>
       <c r="E259" s="25"/>
       <c r="F259" s="25"/>
       <c r="G259" s="25"/>
@@ -8272,28 +8283,28 @@
       <c r="J259" s="25"/>
       <c r="K259" s="25"/>
       <c r="L259" s="25"/>
-      <c r="M259" s="95"/>
-      <c r="N259" s="91"/>
-      <c r="O259" s="91"/>
-      <c r="P259" s="91"/>
-      <c r="Q259" s="91"/>
-      <c r="R259" s="91"/>
-      <c r="S259" s="91"/>
-      <c r="T259" s="91"/>
-      <c r="U259" s="91"/>
-      <c r="V259" s="91"/>
-      <c r="W259" s="91"/>
-      <c r="X259" s="91"/>
-      <c r="Y259" s="91"/>
-      <c r="Z259" s="91"/>
+      <c r="M259" s="96"/>
+      <c r="N259" s="92"/>
+      <c r="O259" s="92"/>
+      <c r="P259" s="92"/>
+      <c r="Q259" s="92"/>
+      <c r="R259" s="92"/>
+      <c r="S259" s="92"/>
+      <c r="T259" s="92"/>
+      <c r="U259" s="92"/>
+      <c r="V259" s="92"/>
+      <c r="W259" s="92"/>
+      <c r="X259" s="92"/>
+      <c r="Y259" s="92"/>
+      <c r="Z259" s="92"/>
     </row>
     <row r="260" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A260" s="91"/>
-      <c r="B260" s="100" t="s">
+      <c r="A260" s="92"/>
+      <c r="B260" s="101" t="s">
         <v>441</v>
       </c>
-      <c r="C260" s="93"/>
-      <c r="D260" s="94"/>
+      <c r="C260" s="94"/>
+      <c r="D260" s="95"/>
       <c r="E260" s="25"/>
       <c r="F260" s="25"/>
       <c r="G260" s="25"/>
@@ -8302,30 +8313,30 @@
       <c r="J260" s="25"/>
       <c r="K260" s="25"/>
       <c r="L260" s="25"/>
-      <c r="M260" s="95"/>
-      <c r="N260" s="91"/>
-      <c r="O260" s="91"/>
-      <c r="P260" s="91"/>
-      <c r="Q260" s="91"/>
-      <c r="R260" s="91"/>
-      <c r="S260" s="91"/>
-      <c r="T260" s="91"/>
-      <c r="U260" s="91"/>
-      <c r="V260" s="91"/>
-      <c r="W260" s="91"/>
-      <c r="X260" s="91"/>
-      <c r="Y260" s="91"/>
-      <c r="Z260" s="91"/>
+      <c r="M260" s="96"/>
+      <c r="N260" s="92"/>
+      <c r="O260" s="92"/>
+      <c r="P260" s="92"/>
+      <c r="Q260" s="92"/>
+      <c r="R260" s="92"/>
+      <c r="S260" s="92"/>
+      <c r="T260" s="92"/>
+      <c r="U260" s="92"/>
+      <c r="V260" s="92"/>
+      <c r="W260" s="92"/>
+      <c r="X260" s="92"/>
+      <c r="Y260" s="92"/>
+      <c r="Z260" s="92"/>
     </row>
     <row r="261" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A261" s="91"/>
-      <c r="B261" s="98" t="s">
+      <c r="A261" s="92"/>
+      <c r="B261" s="99" t="s">
         <v>442</v>
       </c>
-      <c r="C261" s="101" t="s">
+      <c r="C261" s="102" t="s">
         <v>443</v>
       </c>
-      <c r="D261" s="94"/>
+      <c r="D261" s="95"/>
       <c r="E261" s="25"/>
       <c r="F261" s="25"/>
       <c r="G261" s="25"/>
@@ -8338,30 +8349,30 @@
       </c>
       <c r="K261" s="25"/>
       <c r="L261" s="25"/>
-      <c r="M261" s="95"/>
-      <c r="N261" s="91"/>
-      <c r="O261" s="91"/>
-      <c r="P261" s="91"/>
-      <c r="Q261" s="91"/>
-      <c r="R261" s="91"/>
-      <c r="S261" s="91"/>
-      <c r="T261" s="91"/>
-      <c r="U261" s="91"/>
-      <c r="V261" s="91"/>
-      <c r="W261" s="91"/>
-      <c r="X261" s="91"/>
-      <c r="Y261" s="91"/>
-      <c r="Z261" s="91"/>
+      <c r="M261" s="96"/>
+      <c r="N261" s="92"/>
+      <c r="O261" s="92"/>
+      <c r="P261" s="92"/>
+      <c r="Q261" s="92"/>
+      <c r="R261" s="92"/>
+      <c r="S261" s="92"/>
+      <c r="T261" s="92"/>
+      <c r="U261" s="92"/>
+      <c r="V261" s="92"/>
+      <c r="W261" s="92"/>
+      <c r="X261" s="92"/>
+      <c r="Y261" s="92"/>
+      <c r="Z261" s="92"/>
     </row>
     <row r="262" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A262" s="91"/>
-      <c r="B262" s="92" t="s">
+      <c r="A262" s="92"/>
+      <c r="B262" s="93" t="s">
         <v>444</v>
       </c>
-      <c r="C262" s="93" t="s">
+      <c r="C262" s="94" t="s">
         <v>445</v>
       </c>
-      <c r="D262" s="94"/>
+      <c r="D262" s="95"/>
       <c r="E262" s="25"/>
       <c r="F262" s="25"/>
       <c r="G262" s="25"/>
@@ -8370,28 +8381,28 @@
       <c r="J262" s="25"/>
       <c r="K262" s="25"/>
       <c r="L262" s="25"/>
-      <c r="M262" s="95"/>
-      <c r="N262" s="91"/>
-      <c r="O262" s="91"/>
-      <c r="P262" s="91"/>
-      <c r="Q262" s="91"/>
-      <c r="R262" s="91"/>
-      <c r="S262" s="91"/>
-      <c r="T262" s="91"/>
-      <c r="U262" s="91"/>
-      <c r="V262" s="91"/>
-      <c r="W262" s="91"/>
-      <c r="X262" s="91"/>
-      <c r="Y262" s="91"/>
-      <c r="Z262" s="91"/>
+      <c r="M262" s="96"/>
+      <c r="N262" s="92"/>
+      <c r="O262" s="92"/>
+      <c r="P262" s="92"/>
+      <c r="Q262" s="92"/>
+      <c r="R262" s="92"/>
+      <c r="S262" s="92"/>
+      <c r="T262" s="92"/>
+      <c r="U262" s="92"/>
+      <c r="V262" s="92"/>
+      <c r="W262" s="92"/>
+      <c r="X262" s="92"/>
+      <c r="Y262" s="92"/>
+      <c r="Z262" s="92"/>
     </row>
     <row r="263" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A263" s="91"/>
-      <c r="B263" s="100" t="s">
+      <c r="A263" s="92"/>
+      <c r="B263" s="101" t="s">
         <v>446</v>
       </c>
-      <c r="C263" s="93"/>
-      <c r="D263" s="94"/>
+      <c r="C263" s="94"/>
+      <c r="D263" s="95"/>
       <c r="E263" s="25"/>
       <c r="F263" s="25"/>
       <c r="G263" s="25"/>
@@ -8400,30 +8411,30 @@
       <c r="J263" s="25"/>
       <c r="K263" s="25"/>
       <c r="L263" s="25"/>
-      <c r="M263" s="95"/>
-      <c r="N263" s="91"/>
-      <c r="O263" s="91"/>
-      <c r="P263" s="91"/>
-      <c r="Q263" s="91"/>
-      <c r="R263" s="91"/>
-      <c r="S263" s="91"/>
-      <c r="T263" s="91"/>
-      <c r="U263" s="91"/>
-      <c r="V263" s="91"/>
-      <c r="W263" s="91"/>
-      <c r="X263" s="91"/>
-      <c r="Y263" s="91"/>
-      <c r="Z263" s="91"/>
+      <c r="M263" s="96"/>
+      <c r="N263" s="92"/>
+      <c r="O263" s="92"/>
+      <c r="P263" s="92"/>
+      <c r="Q263" s="92"/>
+      <c r="R263" s="92"/>
+      <c r="S263" s="92"/>
+      <c r="T263" s="92"/>
+      <c r="U263" s="92"/>
+      <c r="V263" s="92"/>
+      <c r="W263" s="92"/>
+      <c r="X263" s="92"/>
+      <c r="Y263" s="92"/>
+      <c r="Z263" s="92"/>
     </row>
     <row r="264" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A264" s="91"/>
-      <c r="B264" s="98" t="s">
+      <c r="A264" s="92"/>
+      <c r="B264" s="99" t="s">
         <v>447</v>
       </c>
-      <c r="C264" s="102" t="s">
+      <c r="C264" s="103" t="s">
         <v>448</v>
       </c>
-      <c r="D264" s="94"/>
+      <c r="D264" s="95"/>
       <c r="E264" s="25"/>
       <c r="F264" s="25"/>
       <c r="G264" s="25"/>
@@ -8436,28 +8447,28 @@
       </c>
       <c r="K264" s="25"/>
       <c r="L264" s="25"/>
-      <c r="M264" s="95"/>
-      <c r="N264" s="91"/>
-      <c r="O264" s="91"/>
-      <c r="P264" s="91"/>
-      <c r="Q264" s="91"/>
-      <c r="R264" s="91"/>
-      <c r="S264" s="91"/>
-      <c r="T264" s="91"/>
-      <c r="U264" s="91"/>
-      <c r="V264" s="91"/>
-      <c r="W264" s="91"/>
-      <c r="X264" s="91"/>
-      <c r="Y264" s="91"/>
-      <c r="Z264" s="91"/>
+      <c r="M264" s="96"/>
+      <c r="N264" s="92"/>
+      <c r="O264" s="92"/>
+      <c r="P264" s="92"/>
+      <c r="Q264" s="92"/>
+      <c r="R264" s="92"/>
+      <c r="S264" s="92"/>
+      <c r="T264" s="92"/>
+      <c r="U264" s="92"/>
+      <c r="V264" s="92"/>
+      <c r="W264" s="92"/>
+      <c r="X264" s="92"/>
+      <c r="Y264" s="92"/>
+      <c r="Z264" s="92"/>
     </row>
     <row r="265" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A265" s="91"/>
-      <c r="B265" s="98" t="s">
+      <c r="A265" s="92"/>
+      <c r="B265" s="99" t="s">
         <v>449</v>
       </c>
-      <c r="C265" s="103"/>
-      <c r="D265" s="94"/>
+      <c r="C265" s="104"/>
+      <c r="D265" s="95"/>
       <c r="E265" s="25"/>
       <c r="F265" s="25"/>
       <c r="G265" s="25"/>
@@ -8466,30 +8477,30 @@
       <c r="J265" s="25"/>
       <c r="K265" s="25"/>
       <c r="L265" s="25"/>
-      <c r="M265" s="95"/>
-      <c r="N265" s="91"/>
-      <c r="O265" s="91"/>
-      <c r="P265" s="91"/>
-      <c r="Q265" s="91"/>
-      <c r="R265" s="91"/>
-      <c r="S265" s="91"/>
-      <c r="T265" s="91"/>
-      <c r="U265" s="91"/>
-      <c r="V265" s="91"/>
-      <c r="W265" s="91"/>
-      <c r="X265" s="91"/>
-      <c r="Y265" s="91"/>
-      <c r="Z265" s="91"/>
+      <c r="M265" s="96"/>
+      <c r="N265" s="92"/>
+      <c r="O265" s="92"/>
+      <c r="P265" s="92"/>
+      <c r="Q265" s="92"/>
+      <c r="R265" s="92"/>
+      <c r="S265" s="92"/>
+      <c r="T265" s="92"/>
+      <c r="U265" s="92"/>
+      <c r="V265" s="92"/>
+      <c r="W265" s="92"/>
+      <c r="X265" s="92"/>
+      <c r="Y265" s="92"/>
+      <c r="Z265" s="92"/>
     </row>
     <row r="266" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A266" s="91"/>
-      <c r="B266" s="92" t="s">
+      <c r="A266" s="92"/>
+      <c r="B266" s="93" t="s">
         <v>450</v>
       </c>
-      <c r="C266" s="93" t="s">
+      <c r="C266" s="94" t="s">
         <v>451</v>
       </c>
-      <c r="D266" s="94"/>
+      <c r="D266" s="95"/>
       <c r="E266" s="25"/>
       <c r="F266" s="25"/>
       <c r="G266" s="25"/>
@@ -8498,28 +8509,28 @@
       <c r="J266" s="25"/>
       <c r="K266" s="25"/>
       <c r="L266" s="25"/>
-      <c r="M266" s="95"/>
-      <c r="N266" s="91"/>
-      <c r="O266" s="91"/>
-      <c r="P266" s="91"/>
-      <c r="Q266" s="91"/>
-      <c r="R266" s="91"/>
-      <c r="S266" s="91"/>
-      <c r="T266" s="91"/>
-      <c r="U266" s="91"/>
-      <c r="V266" s="91"/>
-      <c r="W266" s="91"/>
-      <c r="X266" s="91"/>
-      <c r="Y266" s="91"/>
-      <c r="Z266" s="91"/>
+      <c r="M266" s="96"/>
+      <c r="N266" s="92"/>
+      <c r="O266" s="92"/>
+      <c r="P266" s="92"/>
+      <c r="Q266" s="92"/>
+      <c r="R266" s="92"/>
+      <c r="S266" s="92"/>
+      <c r="T266" s="92"/>
+      <c r="U266" s="92"/>
+      <c r="V266" s="92"/>
+      <c r="W266" s="92"/>
+      <c r="X266" s="92"/>
+      <c r="Y266" s="92"/>
+      <c r="Z266" s="92"/>
     </row>
     <row r="267" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A267" s="91"/>
-      <c r="B267" s="96" t="s">
+      <c r="A267" s="92"/>
+      <c r="B267" s="97" t="s">
         <v>452</v>
       </c>
-      <c r="C267" s="104"/>
-      <c r="D267" s="94"/>
+      <c r="C267" s="105"/>
+      <c r="D267" s="95"/>
       <c r="E267" s="25"/>
       <c r="F267" s="25"/>
       <c r="G267" s="25"/>
@@ -8528,28 +8539,28 @@
       <c r="J267" s="25"/>
       <c r="K267" s="25"/>
       <c r="L267" s="25"/>
-      <c r="M267" s="95"/>
-      <c r="N267" s="91"/>
-      <c r="O267" s="91"/>
-      <c r="P267" s="91"/>
-      <c r="Q267" s="91"/>
-      <c r="R267" s="91"/>
-      <c r="S267" s="91"/>
-      <c r="T267" s="91"/>
-      <c r="U267" s="91"/>
-      <c r="V267" s="91"/>
-      <c r="W267" s="91"/>
-      <c r="X267" s="91"/>
-      <c r="Y267" s="91"/>
-      <c r="Z267" s="91"/>
+      <c r="M267" s="96"/>
+      <c r="N267" s="92"/>
+      <c r="O267" s="92"/>
+      <c r="P267" s="92"/>
+      <c r="Q267" s="92"/>
+      <c r="R267" s="92"/>
+      <c r="S267" s="92"/>
+      <c r="T267" s="92"/>
+      <c r="U267" s="92"/>
+      <c r="V267" s="92"/>
+      <c r="W267" s="92"/>
+      <c r="X267" s="92"/>
+      <c r="Y267" s="92"/>
+      <c r="Z267" s="92"/>
     </row>
     <row r="268" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A268" s="91"/>
-      <c r="B268" s="97"/>
-      <c r="C268" s="99" t="s">
+      <c r="A268" s="92"/>
+      <c r="B268" s="98"/>
+      <c r="C268" s="100" t="s">
         <v>453</v>
       </c>
-      <c r="D268" s="94"/>
+      <c r="D268" s="95"/>
       <c r="E268" s="25"/>
       <c r="F268" s="25"/>
       <c r="G268" s="25"/>
@@ -8562,30 +8573,30 @@
       </c>
       <c r="K268" s="25"/>
       <c r="L268" s="25"/>
-      <c r="M268" s="95"/>
-      <c r="N268" s="91"/>
-      <c r="O268" s="91"/>
-      <c r="P268" s="91"/>
-      <c r="Q268" s="91"/>
-      <c r="R268" s="91"/>
-      <c r="S268" s="91"/>
-      <c r="T268" s="91"/>
-      <c r="U268" s="91"/>
-      <c r="V268" s="91"/>
-      <c r="W268" s="91"/>
-      <c r="X268" s="91"/>
-      <c r="Y268" s="91"/>
-      <c r="Z268" s="91"/>
+      <c r="M268" s="96"/>
+      <c r="N268" s="92"/>
+      <c r="O268" s="92"/>
+      <c r="P268" s="92"/>
+      <c r="Q268" s="92"/>
+      <c r="R268" s="92"/>
+      <c r="S268" s="92"/>
+      <c r="T268" s="92"/>
+      <c r="U268" s="92"/>
+      <c r="V268" s="92"/>
+      <c r="W268" s="92"/>
+      <c r="X268" s="92"/>
+      <c r="Y268" s="92"/>
+      <c r="Z268" s="92"/>
     </row>
     <row r="269" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A269" s="91"/>
-      <c r="B269" s="92" t="s">
+      <c r="A269" s="92"/>
+      <c r="B269" s="93" t="s">
         <v>454</v>
       </c>
-      <c r="C269" s="93" t="s">
+      <c r="C269" s="94" t="s">
         <v>455</v>
       </c>
-      <c r="D269" s="94"/>
+      <c r="D269" s="95"/>
       <c r="E269" s="25"/>
       <c r="F269" s="25"/>
       <c r="G269" s="25"/>
@@ -8594,28 +8605,28 @@
       <c r="J269" s="25"/>
       <c r="K269" s="25"/>
       <c r="L269" s="25"/>
-      <c r="M269" s="95"/>
-      <c r="N269" s="91"/>
-      <c r="O269" s="91"/>
-      <c r="P269" s="91"/>
-      <c r="Q269" s="91"/>
-      <c r="R269" s="91"/>
-      <c r="S269" s="91"/>
-      <c r="T269" s="91"/>
-      <c r="U269" s="91"/>
-      <c r="V269" s="91"/>
-      <c r="W269" s="91"/>
-      <c r="X269" s="91"/>
-      <c r="Y269" s="91"/>
-      <c r="Z269" s="91"/>
+      <c r="M269" s="96"/>
+      <c r="N269" s="92"/>
+      <c r="O269" s="92"/>
+      <c r="P269" s="92"/>
+      <c r="Q269" s="92"/>
+      <c r="R269" s="92"/>
+      <c r="S269" s="92"/>
+      <c r="T269" s="92"/>
+      <c r="U269" s="92"/>
+      <c r="V269" s="92"/>
+      <c r="W269" s="92"/>
+      <c r="X269" s="92"/>
+      <c r="Y269" s="92"/>
+      <c r="Z269" s="92"/>
     </row>
     <row r="270" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A270" s="91"/>
-      <c r="B270" s="96" t="s">
+      <c r="A270" s="92"/>
+      <c r="B270" s="97" t="s">
         <v>456</v>
       </c>
-      <c r="C270" s="93"/>
-      <c r="D270" s="94"/>
+      <c r="C270" s="94"/>
+      <c r="D270" s="95"/>
       <c r="E270" s="25"/>
       <c r="F270" s="25"/>
       <c r="G270" s="25"/>
@@ -8624,28 +8635,28 @@
       <c r="J270" s="25"/>
       <c r="K270" s="25"/>
       <c r="L270" s="25"/>
-      <c r="M270" s="95"/>
-      <c r="N270" s="91"/>
-      <c r="O270" s="91"/>
-      <c r="P270" s="91"/>
-      <c r="Q270" s="91"/>
-      <c r="R270" s="91"/>
-      <c r="S270" s="91"/>
-      <c r="T270" s="91"/>
-      <c r="U270" s="91"/>
-      <c r="V270" s="91"/>
-      <c r="W270" s="91"/>
-      <c r="X270" s="91"/>
-      <c r="Y270" s="91"/>
-      <c r="Z270" s="91"/>
+      <c r="M270" s="96"/>
+      <c r="N270" s="92"/>
+      <c r="O270" s="92"/>
+      <c r="P270" s="92"/>
+      <c r="Q270" s="92"/>
+      <c r="R270" s="92"/>
+      <c r="S270" s="92"/>
+      <c r="T270" s="92"/>
+      <c r="U270" s="92"/>
+      <c r="V270" s="92"/>
+      <c r="W270" s="92"/>
+      <c r="X270" s="92"/>
+      <c r="Y270" s="92"/>
+      <c r="Z270" s="92"/>
     </row>
     <row r="271" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A271" s="91"/>
-      <c r="B271" s="97"/>
-      <c r="C271" s="99" t="s">
+      <c r="A271" s="92"/>
+      <c r="B271" s="98"/>
+      <c r="C271" s="100" t="s">
         <v>457</v>
       </c>
-      <c r="D271" s="94"/>
+      <c r="D271" s="95"/>
       <c r="E271" s="25"/>
       <c r="F271" s="25"/>
       <c r="G271" s="25"/>
@@ -8658,30 +8669,30 @@
       </c>
       <c r="K271" s="25"/>
       <c r="L271" s="25"/>
-      <c r="M271" s="95"/>
-      <c r="N271" s="91"/>
-      <c r="O271" s="91"/>
-      <c r="P271" s="91"/>
-      <c r="Q271" s="91"/>
-      <c r="R271" s="91"/>
-      <c r="S271" s="91"/>
-      <c r="T271" s="91"/>
-      <c r="U271" s="91"/>
-      <c r="V271" s="91"/>
-      <c r="W271" s="91"/>
-      <c r="X271" s="91"/>
-      <c r="Y271" s="91"/>
-      <c r="Z271" s="91"/>
+      <c r="M271" s="96"/>
+      <c r="N271" s="92"/>
+      <c r="O271" s="92"/>
+      <c r="P271" s="92"/>
+      <c r="Q271" s="92"/>
+      <c r="R271" s="92"/>
+      <c r="S271" s="92"/>
+      <c r="T271" s="92"/>
+      <c r="U271" s="92"/>
+      <c r="V271" s="92"/>
+      <c r="W271" s="92"/>
+      <c r="X271" s="92"/>
+      <c r="Y271" s="92"/>
+      <c r="Z271" s="92"/>
     </row>
     <row r="272" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A272" s="91"/>
-      <c r="B272" s="92" t="s">
+      <c r="A272" s="92"/>
+      <c r="B272" s="93" t="s">
         <v>458</v>
       </c>
-      <c r="C272" s="93" t="s">
+      <c r="C272" s="94" t="s">
         <v>459</v>
       </c>
-      <c r="D272" s="94"/>
+      <c r="D272" s="95"/>
       <c r="E272" s="25"/>
       <c r="F272" s="25"/>
       <c r="G272" s="25"/>
@@ -8690,28 +8701,28 @@
       <c r="J272" s="25"/>
       <c r="K272" s="25"/>
       <c r="L272" s="25"/>
-      <c r="M272" s="95"/>
-      <c r="N272" s="91"/>
-      <c r="O272" s="91"/>
-      <c r="P272" s="91"/>
-      <c r="Q272" s="91"/>
-      <c r="R272" s="91"/>
-      <c r="S272" s="91"/>
-      <c r="T272" s="91"/>
-      <c r="U272" s="91"/>
-      <c r="V272" s="91"/>
-      <c r="W272" s="91"/>
-      <c r="X272" s="91"/>
-      <c r="Y272" s="91"/>
-      <c r="Z272" s="91"/>
+      <c r="M272" s="96"/>
+      <c r="N272" s="92"/>
+      <c r="O272" s="92"/>
+      <c r="P272" s="92"/>
+      <c r="Q272" s="92"/>
+      <c r="R272" s="92"/>
+      <c r="S272" s="92"/>
+      <c r="T272" s="92"/>
+      <c r="U272" s="92"/>
+      <c r="V272" s="92"/>
+      <c r="W272" s="92"/>
+      <c r="X272" s="92"/>
+      <c r="Y272" s="92"/>
+      <c r="Z272" s="92"/>
     </row>
     <row r="273" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A273" s="91"/>
-      <c r="B273" s="100" t="s">
+      <c r="A273" s="92"/>
+      <c r="B273" s="101" t="s">
         <v>460</v>
       </c>
-      <c r="C273" s="93"/>
-      <c r="D273" s="94"/>
+      <c r="C273" s="94"/>
+      <c r="D273" s="95"/>
       <c r="E273" s="25"/>
       <c r="F273" s="25"/>
       <c r="G273" s="25"/>
@@ -8720,30 +8731,30 @@
       <c r="J273" s="25"/>
       <c r="K273" s="25"/>
       <c r="L273" s="25"/>
-      <c r="M273" s="95"/>
-      <c r="N273" s="91"/>
-      <c r="O273" s="91"/>
-      <c r="P273" s="91"/>
-      <c r="Q273" s="91"/>
-      <c r="R273" s="91"/>
-      <c r="S273" s="91"/>
-      <c r="T273" s="91"/>
-      <c r="U273" s="91"/>
-      <c r="V273" s="91"/>
-      <c r="W273" s="91"/>
-      <c r="X273" s="91"/>
-      <c r="Y273" s="91"/>
-      <c r="Z273" s="91"/>
+      <c r="M273" s="96"/>
+      <c r="N273" s="92"/>
+      <c r="O273" s="92"/>
+      <c r="P273" s="92"/>
+      <c r="Q273" s="92"/>
+      <c r="R273" s="92"/>
+      <c r="S273" s="92"/>
+      <c r="T273" s="92"/>
+      <c r="U273" s="92"/>
+      <c r="V273" s="92"/>
+      <c r="W273" s="92"/>
+      <c r="X273" s="92"/>
+      <c r="Y273" s="92"/>
+      <c r="Z273" s="92"/>
     </row>
     <row r="274" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A274" s="91"/>
-      <c r="B274" s="98" t="s">
+      <c r="A274" s="92"/>
+      <c r="B274" s="99" t="s">
         <v>461</v>
       </c>
-      <c r="C274" s="99" t="s">
+      <c r="C274" s="100" t="s">
         <v>462</v>
       </c>
-      <c r="D274" s="94"/>
+      <c r="D274" s="95"/>
       <c r="E274" s="25"/>
       <c r="F274" s="25"/>
       <c r="G274" s="25"/>
@@ -8756,30 +8767,30 @@
       </c>
       <c r="K274" s="25"/>
       <c r="L274" s="25"/>
-      <c r="M274" s="95"/>
-      <c r="N274" s="91"/>
-      <c r="O274" s="91"/>
-      <c r="P274" s="91"/>
-      <c r="Q274" s="91"/>
-      <c r="R274" s="91"/>
-      <c r="S274" s="91"/>
-      <c r="T274" s="91"/>
-      <c r="U274" s="91"/>
-      <c r="V274" s="91"/>
-      <c r="W274" s="91"/>
-      <c r="X274" s="91"/>
-      <c r="Y274" s="91"/>
-      <c r="Z274" s="91"/>
+      <c r="M274" s="96"/>
+      <c r="N274" s="92"/>
+      <c r="O274" s="92"/>
+      <c r="P274" s="92"/>
+      <c r="Q274" s="92"/>
+      <c r="R274" s="92"/>
+      <c r="S274" s="92"/>
+      <c r="T274" s="92"/>
+      <c r="U274" s="92"/>
+      <c r="V274" s="92"/>
+      <c r="W274" s="92"/>
+      <c r="X274" s="92"/>
+      <c r="Y274" s="92"/>
+      <c r="Z274" s="92"/>
     </row>
     <row r="275" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A275" s="91"/>
-      <c r="B275" s="92" t="s">
+      <c r="A275" s="92"/>
+      <c r="B275" s="93" t="s">
         <v>463</v>
       </c>
-      <c r="C275" s="93" t="s">
+      <c r="C275" s="94" t="s">
         <v>464</v>
       </c>
-      <c r="D275" s="94"/>
+      <c r="D275" s="95"/>
       <c r="E275" s="25"/>
       <c r="F275" s="25"/>
       <c r="G275" s="25"/>
@@ -8788,28 +8799,28 @@
       <c r="J275" s="25"/>
       <c r="K275" s="25"/>
       <c r="L275" s="25"/>
-      <c r="M275" s="95"/>
-      <c r="N275" s="91"/>
-      <c r="O275" s="91"/>
-      <c r="P275" s="91"/>
-      <c r="Q275" s="91"/>
-      <c r="R275" s="91"/>
-      <c r="S275" s="91"/>
-      <c r="T275" s="91"/>
-      <c r="U275" s="91"/>
-      <c r="V275" s="91"/>
-      <c r="W275" s="91"/>
-      <c r="X275" s="91"/>
-      <c r="Y275" s="91"/>
-      <c r="Z275" s="91"/>
+      <c r="M275" s="96"/>
+      <c r="N275" s="92"/>
+      <c r="O275" s="92"/>
+      <c r="P275" s="92"/>
+      <c r="Q275" s="92"/>
+      <c r="R275" s="92"/>
+      <c r="S275" s="92"/>
+      <c r="T275" s="92"/>
+      <c r="U275" s="92"/>
+      <c r="V275" s="92"/>
+      <c r="W275" s="92"/>
+      <c r="X275" s="92"/>
+      <c r="Y275" s="92"/>
+      <c r="Z275" s="92"/>
     </row>
     <row r="276" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A276" s="91"/>
-      <c r="B276" s="100" t="s">
+      <c r="A276" s="92"/>
+      <c r="B276" s="101" t="s">
         <v>465</v>
       </c>
-      <c r="C276" s="93"/>
-      <c r="D276" s="94"/>
+      <c r="C276" s="94"/>
+      <c r="D276" s="95"/>
       <c r="E276" s="25"/>
       <c r="F276" s="25"/>
       <c r="G276" s="25"/>
@@ -8818,30 +8829,30 @@
       <c r="J276" s="25"/>
       <c r="K276" s="25"/>
       <c r="L276" s="25"/>
-      <c r="M276" s="95"/>
-      <c r="N276" s="91"/>
-      <c r="O276" s="91"/>
-      <c r="P276" s="91"/>
-      <c r="Q276" s="91"/>
-      <c r="R276" s="91"/>
-      <c r="S276" s="91"/>
-      <c r="T276" s="91"/>
-      <c r="U276" s="91"/>
-      <c r="V276" s="91"/>
-      <c r="W276" s="91"/>
-      <c r="X276" s="91"/>
-      <c r="Y276" s="91"/>
-      <c r="Z276" s="91"/>
+      <c r="M276" s="96"/>
+      <c r="N276" s="92"/>
+      <c r="O276" s="92"/>
+      <c r="P276" s="92"/>
+      <c r="Q276" s="92"/>
+      <c r="R276" s="92"/>
+      <c r="S276" s="92"/>
+      <c r="T276" s="92"/>
+      <c r="U276" s="92"/>
+      <c r="V276" s="92"/>
+      <c r="W276" s="92"/>
+      <c r="X276" s="92"/>
+      <c r="Y276" s="92"/>
+      <c r="Z276" s="92"/>
     </row>
     <row r="277" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A277" s="91"/>
-      <c r="B277" s="98" t="s">
+      <c r="A277" s="92"/>
+      <c r="B277" s="99" t="s">
         <v>466</v>
       </c>
-      <c r="C277" s="102" t="s">
+      <c r="C277" s="103" t="s">
         <v>467</v>
       </c>
-      <c r="D277" s="94"/>
+      <c r="D277" s="95"/>
       <c r="E277" s="25"/>
       <c r="F277" s="25"/>
       <c r="G277" s="25"/>
@@ -8850,28 +8861,28 @@
       <c r="J277" s="25"/>
       <c r="K277" s="25"/>
       <c r="L277" s="25"/>
-      <c r="M277" s="95"/>
-      <c r="N277" s="91"/>
-      <c r="O277" s="91"/>
-      <c r="P277" s="91"/>
-      <c r="Q277" s="91"/>
-      <c r="R277" s="91"/>
-      <c r="S277" s="91"/>
-      <c r="T277" s="91"/>
-      <c r="U277" s="91"/>
-      <c r="V277" s="91"/>
-      <c r="W277" s="91"/>
-      <c r="X277" s="91"/>
-      <c r="Y277" s="91"/>
-      <c r="Z277" s="91"/>
+      <c r="M277" s="96"/>
+      <c r="N277" s="92"/>
+      <c r="O277" s="92"/>
+      <c r="P277" s="92"/>
+      <c r="Q277" s="92"/>
+      <c r="R277" s="92"/>
+      <c r="S277" s="92"/>
+      <c r="T277" s="92"/>
+      <c r="U277" s="92"/>
+      <c r="V277" s="92"/>
+      <c r="W277" s="92"/>
+      <c r="X277" s="92"/>
+      <c r="Y277" s="92"/>
+      <c r="Z277" s="92"/>
     </row>
     <row r="278" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A278" s="91"/>
-      <c r="B278" s="98" t="s">
+      <c r="A278" s="92"/>
+      <c r="B278" s="99" t="s">
         <v>468</v>
       </c>
-      <c r="C278" s="103"/>
-      <c r="D278" s="94"/>
+      <c r="C278" s="104"/>
+      <c r="D278" s="95"/>
       <c r="E278" s="25"/>
       <c r="F278" s="25"/>
       <c r="G278" s="25"/>
@@ -8884,20 +8895,20 @@
       </c>
       <c r="K278" s="25"/>
       <c r="L278" s="25"/>
-      <c r="M278" s="95"/>
-      <c r="N278" s="91"/>
-      <c r="O278" s="91"/>
-      <c r="P278" s="91"/>
-      <c r="Q278" s="91"/>
-      <c r="R278" s="91"/>
-      <c r="S278" s="91"/>
-      <c r="T278" s="91"/>
-      <c r="U278" s="91"/>
-      <c r="V278" s="91"/>
-      <c r="W278" s="91"/>
-      <c r="X278" s="91"/>
-      <c r="Y278" s="91"/>
-      <c r="Z278" s="91"/>
+      <c r="M278" s="96"/>
+      <c r="N278" s="92"/>
+      <c r="O278" s="92"/>
+      <c r="P278" s="92"/>
+      <c r="Q278" s="92"/>
+      <c r="R278" s="92"/>
+      <c r="S278" s="92"/>
+      <c r="T278" s="92"/>
+      <c r="U278" s="92"/>
+      <c r="V278" s="92"/>
+      <c r="W278" s="92"/>
+      <c r="X278" s="92"/>
+      <c r="Y278" s="92"/>
+      <c r="Z278" s="92"/>
     </row>
     <row r="279" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B279" s="18" t="s">
@@ -8919,7 +8930,7 @@
       <c r="A280" s="26" t="s">
         <v>470</v>
       </c>
-      <c r="B280" s="88" t="s">
+      <c r="B280" s="89" t="s">
         <v>471</v>
       </c>
       <c r="C280" s="80" t="s">
@@ -8985,7 +8996,7 @@
     </row>
     <row r="283" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B283" s="53"/>
-      <c r="C283" s="105" t="s">
+      <c r="C283" s="106" t="s">
         <v>476</v>
       </c>
       <c r="D283" s="81"/>
@@ -9001,7 +9012,7 @@
     </row>
     <row r="284" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B284" s="53"/>
-      <c r="C284" s="105" t="s">
+      <c r="C284" s="106" t="s">
         <v>477</v>
       </c>
       <c r="D284" s="81"/>
@@ -9017,7 +9028,7 @@
     </row>
     <row r="285" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B285" s="31"/>
-      <c r="C285" s="106" t="s">
+      <c r="C285" s="107" t="s">
         <v>478</v>
       </c>
       <c r="D285" s="81"/>
@@ -9035,7 +9046,7 @@
       <c r="A286" s="83" t="s">
         <v>479</v>
       </c>
-      <c r="B286" s="88" t="s">
+      <c r="B286" s="89" t="s">
         <v>480</v>
       </c>
       <c r="C286" s="80" t="s">
@@ -9103,13 +9114,13 @@
       <c r="A289" s="26" t="s">
         <v>485</v>
       </c>
-      <c r="B289" s="88" t="s">
+      <c r="B289" s="89" t="s">
         <v>486</v>
       </c>
       <c r="C289" s="80" t="s">
         <v>487</v>
       </c>
-      <c r="D289" s="107" t="s">
+      <c r="D289" s="108" t="s">
         <v>488</v>
       </c>
       <c r="E289" s="22" t="n">
@@ -9231,11 +9242,11 @@
       <c r="A295" s="26" t="s">
         <v>494</v>
       </c>
-      <c r="B295" s="88" t="s">
+      <c r="B295" s="89" t="s">
         <v>495</v>
       </c>
-      <c r="C295" s="108"/>
-      <c r="D295" s="107" t="s">
+      <c r="C295" s="109"/>
+      <c r="D295" s="108" t="s">
         <v>496</v>
       </c>
       <c r="E295" s="22" t="n">
@@ -9273,7 +9284,7 @@
       <c r="B296" s="30" t="s">
         <v>498</v>
       </c>
-      <c r="C296" s="108"/>
+      <c r="C296" s="109"/>
       <c r="D296" s="44"/>
       <c r="E296" s="17"/>
       <c r="F296" s="17"/>
@@ -9287,7 +9298,7 @@
     </row>
     <row r="297" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B297" s="31"/>
-      <c r="C297" s="108"/>
+      <c r="C297" s="109"/>
       <c r="D297" s="33" t="s">
         <v>499</v>
       </c>
@@ -9305,7 +9316,7 @@
       <c r="A298" s="26" t="s">
         <v>500</v>
       </c>
-      <c r="B298" s="88" t="s">
+      <c r="B298" s="89" t="s">
         <v>501</v>
       </c>
       <c r="C298" s="80" t="s">
@@ -9375,13 +9386,13 @@
     </row>
     <row r="301" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A301" s="83"/>
-      <c r="B301" s="88" t="s">
+      <c r="B301" s="89" t="s">
         <v>506</v>
       </c>
       <c r="C301" s="80" t="s">
         <v>507</v>
       </c>
-      <c r="D301" s="107" t="s">
+      <c r="D301" s="108" t="s">
         <v>507</v>
       </c>
       <c r="E301" s="22"/>
@@ -17213,7 +17224,7 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:N25"/>
+  <dimension ref="A1:N1000"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
@@ -17234,424 +17245,424 @@
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="109" t="s">
+      <c r="A4" s="110" t="s">
         <v>511</v>
       </c>
-      <c r="B4" s="110"/>
-      <c r="C4" s="110"/>
-      <c r="D4" s="110"/>
-      <c r="E4" s="110"/>
-      <c r="F4" s="110"/>
-      <c r="G4" s="110"/>
-      <c r="H4" s="110"/>
-      <c r="I4" s="110"/>
-      <c r="J4" s="110"/>
-      <c r="K4" s="110"/>
-      <c r="L4" s="110"/>
-      <c r="M4" s="110"/>
-      <c r="N4" s="110"/>
+      <c r="B4" s="111"/>
+      <c r="C4" s="111"/>
+      <c r="D4" s="111"/>
+      <c r="E4" s="111"/>
+      <c r="F4" s="111"/>
+      <c r="G4" s="111"/>
+      <c r="H4" s="111"/>
+      <c r="I4" s="111"/>
+      <c r="J4" s="111"/>
+      <c r="K4" s="111"/>
+      <c r="L4" s="111"/>
+      <c r="M4" s="111"/>
+      <c r="N4" s="111"/>
     </row>
     <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="109" t="s">
+      <c r="A5" s="110" t="s">
         <v>512</v>
       </c>
-      <c r="B5" s="111" t="s">
+      <c r="B5" s="112" t="s">
         <v>513</v>
       </c>
-      <c r="C5" s="109" t="s">
+      <c r="C5" s="110" t="s">
         <v>514</v>
       </c>
-      <c r="D5" s="111" t="s">
+      <c r="D5" s="112" t="s">
         <v>515</v>
       </c>
-      <c r="E5" s="111" t="s">
+      <c r="E5" s="112" t="s">
         <v>516</v>
       </c>
-      <c r="F5" s="111" t="s">
+      <c r="F5" s="112" t="s">
         <v>517</v>
       </c>
-      <c r="G5" s="111" t="s">
+      <c r="G5" s="112" t="s">
         <v>518</v>
       </c>
-      <c r="H5" s="111" t="s">
+      <c r="H5" s="112" t="s">
         <v>519</v>
       </c>
-      <c r="I5" s="111" t="s">
+      <c r="I5" s="112" t="s">
         <v>520</v>
       </c>
-      <c r="J5" s="111" t="s">
+      <c r="J5" s="112" t="s">
         <v>521</v>
       </c>
-      <c r="K5" s="111" t="s">
+      <c r="K5" s="112" t="s">
         <v>522</v>
       </c>
-      <c r="L5" s="111" t="s">
+      <c r="L5" s="112" t="s">
         <v>523</v>
       </c>
-      <c r="M5" s="111" t="s">
+      <c r="M5" s="112" t="s">
         <v>524</v>
       </c>
-      <c r="N5" s="109" t="s">
+      <c r="N5" s="110" t="s">
         <v>525</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="112" t="s">
+      <c r="A6" s="113" t="s">
         <v>526</v>
       </c>
-      <c r="B6" s="113" t="n">
+      <c r="B6" s="114" t="n">
         <v>180</v>
       </c>
-      <c r="C6" s="112" t="s">
+      <c r="C6" s="113" t="s">
         <v>527</v>
       </c>
-      <c r="D6" s="114"/>
-      <c r="E6" s="114"/>
-      <c r="F6" s="114"/>
-      <c r="G6" s="114"/>
-      <c r="H6" s="114"/>
-      <c r="I6" s="113" t="n">
+      <c r="D6" s="115"/>
+      <c r="E6" s="115"/>
+      <c r="F6" s="115"/>
+      <c r="G6" s="115"/>
+      <c r="H6" s="115"/>
+      <c r="I6" s="114" t="n">
         <v>280</v>
       </c>
-      <c r="J6" s="113" t="n">
+      <c r="J6" s="114" t="n">
         <v>330</v>
       </c>
-      <c r="K6" s="114"/>
-      <c r="L6" s="114"/>
-      <c r="M6" s="114"/>
-      <c r="N6" s="112"/>
+      <c r="K6" s="115"/>
+      <c r="L6" s="115"/>
+      <c r="M6" s="115"/>
+      <c r="N6" s="113"/>
     </row>
     <row r="7" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="110" t="s">
+      <c r="A7" s="111" t="s">
         <v>526</v>
       </c>
-      <c r="B7" s="115" t="n">
+      <c r="B7" s="116" t="n">
         <v>365</v>
       </c>
-      <c r="C7" s="110" t="s">
+      <c r="C7" s="111" t="s">
         <v>528</v>
       </c>
-      <c r="D7" s="116"/>
-      <c r="E7" s="116"/>
-      <c r="F7" s="116"/>
-      <c r="G7" s="116"/>
-      <c r="H7" s="116"/>
-      <c r="I7" s="115" t="n">
+      <c r="D7" s="117"/>
+      <c r="E7" s="117"/>
+      <c r="F7" s="117"/>
+      <c r="G7" s="117"/>
+      <c r="H7" s="117"/>
+      <c r="I7" s="116" t="n">
         <v>180</v>
       </c>
-      <c r="J7" s="115" t="n">
+      <c r="J7" s="116" t="n">
         <v>210</v>
       </c>
-      <c r="K7" s="116"/>
-      <c r="L7" s="116"/>
-      <c r="M7" s="116"/>
-      <c r="N7" s="110"/>
+      <c r="K7" s="117"/>
+      <c r="L7" s="117"/>
+      <c r="M7" s="117"/>
+      <c r="N7" s="111"/>
     </row>
     <row r="8" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="117" t="s">
+      <c r="A8" s="118" t="s">
         <v>526</v>
       </c>
-      <c r="B8" s="118" t="n">
+      <c r="B8" s="119" t="n">
         <v>1460</v>
       </c>
-      <c r="C8" s="117" t="s">
+      <c r="C8" s="118" t="s">
         <v>529</v>
       </c>
-      <c r="D8" s="119"/>
-      <c r="E8" s="119"/>
-      <c r="F8" s="119"/>
-      <c r="G8" s="119"/>
-      <c r="H8" s="119"/>
-      <c r="I8" s="118" t="n">
+      <c r="D8" s="120"/>
+      <c r="E8" s="120"/>
+      <c r="F8" s="120"/>
+      <c r="G8" s="120"/>
+      <c r="H8" s="120"/>
+      <c r="I8" s="119" t="n">
         <v>75</v>
       </c>
-      <c r="J8" s="118" t="n">
+      <c r="J8" s="119" t="n">
         <v>90</v>
       </c>
-      <c r="K8" s="119"/>
-      <c r="L8" s="119"/>
-      <c r="M8" s="119"/>
-      <c r="N8" s="117"/>
+      <c r="K8" s="120"/>
+      <c r="L8" s="120"/>
+      <c r="M8" s="120"/>
+      <c r="N8" s="118"/>
     </row>
     <row r="9" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="110" t="s">
+      <c r="A9" s="111" t="s">
         <v>530</v>
       </c>
-      <c r="B9" s="115" t="n">
+      <c r="B9" s="116" t="n">
         <v>180</v>
       </c>
-      <c r="C9" s="110" t="s">
+      <c r="C9" s="111" t="s">
         <v>527</v>
       </c>
-      <c r="D9" s="116"/>
-      <c r="E9" s="116"/>
-      <c r="F9" s="116"/>
-      <c r="G9" s="116"/>
-      <c r="H9" s="116"/>
-      <c r="I9" s="115" t="n">
+      <c r="D9" s="117"/>
+      <c r="E9" s="117"/>
+      <c r="F9" s="117"/>
+      <c r="G9" s="117"/>
+      <c r="H9" s="117"/>
+      <c r="I9" s="116" t="n">
         <v>280</v>
       </c>
-      <c r="J9" s="115" t="n">
+      <c r="J9" s="116" t="n">
         <v>330</v>
       </c>
-      <c r="K9" s="116"/>
-      <c r="L9" s="116"/>
-      <c r="M9" s="116"/>
-      <c r="N9" s="110"/>
+      <c r="K9" s="117"/>
+      <c r="L9" s="117"/>
+      <c r="M9" s="117"/>
+      <c r="N9" s="111"/>
     </row>
     <row r="10" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="117" t="s">
+      <c r="A10" s="118" t="s">
         <v>530</v>
       </c>
-      <c r="B10" s="118" t="n">
+      <c r="B10" s="119" t="n">
         <v>365</v>
       </c>
-      <c r="C10" s="117" t="s">
+      <c r="C10" s="118" t="s">
         <v>528</v>
       </c>
-      <c r="D10" s="119"/>
-      <c r="E10" s="119"/>
-      <c r="F10" s="119"/>
-      <c r="G10" s="119"/>
-      <c r="H10" s="119"/>
-      <c r="I10" s="118" t="n">
+      <c r="D10" s="120"/>
+      <c r="E10" s="120"/>
+      <c r="F10" s="120"/>
+      <c r="G10" s="120"/>
+      <c r="H10" s="120"/>
+      <c r="I10" s="119" t="n">
         <v>180</v>
       </c>
-      <c r="J10" s="118" t="n">
+      <c r="J10" s="119" t="n">
         <v>210</v>
       </c>
-      <c r="K10" s="119"/>
-      <c r="L10" s="119"/>
-      <c r="M10" s="119"/>
-      <c r="N10" s="117"/>
+      <c r="K10" s="120"/>
+      <c r="L10" s="120"/>
+      <c r="M10" s="120"/>
+      <c r="N10" s="118"/>
     </row>
     <row r="11" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A11" s="110" t="s">
+      <c r="A11" s="111" t="s">
         <v>530</v>
       </c>
-      <c r="B11" s="115" t="n">
+      <c r="B11" s="116" t="n">
         <v>1460</v>
       </c>
-      <c r="C11" s="110" t="s">
+      <c r="C11" s="111" t="s">
         <v>529</v>
       </c>
-      <c r="D11" s="116"/>
-      <c r="E11" s="116"/>
-      <c r="F11" s="116"/>
-      <c r="G11" s="116"/>
-      <c r="H11" s="116"/>
-      <c r="I11" s="115" t="n">
+      <c r="D11" s="117"/>
+      <c r="E11" s="117"/>
+      <c r="F11" s="117"/>
+      <c r="G11" s="117"/>
+      <c r="H11" s="117"/>
+      <c r="I11" s="116" t="n">
         <v>75</v>
       </c>
-      <c r="J11" s="115" t="n">
+      <c r="J11" s="116" t="n">
         <v>90</v>
       </c>
-      <c r="K11" s="116"/>
-      <c r="L11" s="116"/>
-      <c r="M11" s="116"/>
-      <c r="N11" s="110"/>
+      <c r="K11" s="117"/>
+      <c r="L11" s="117"/>
+      <c r="M11" s="117"/>
+      <c r="N11" s="111"/>
     </row>
     <row r="12" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A12" s="117" t="s">
+      <c r="A12" s="118" t="s">
         <v>526</v>
       </c>
-      <c r="B12" s="118" t="n">
+      <c r="B12" s="119" t="n">
         <v>65535</v>
       </c>
-      <c r="C12" s="117" t="s">
+      <c r="C12" s="118" t="s">
         <v>531</v>
       </c>
-      <c r="D12" s="119"/>
-      <c r="E12" s="119"/>
-      <c r="F12" s="119"/>
-      <c r="G12" s="119"/>
-      <c r="H12" s="119"/>
-      <c r="I12" s="118" t="n">
+      <c r="D12" s="120"/>
+      <c r="E12" s="120"/>
+      <c r="F12" s="120"/>
+      <c r="G12" s="120"/>
+      <c r="H12" s="120"/>
+      <c r="I12" s="119" t="n">
         <v>50</v>
       </c>
-      <c r="J12" s="118" t="n">
+      <c r="J12" s="119" t="n">
         <v>65</v>
       </c>
-      <c r="K12" s="119"/>
-      <c r="L12" s="119"/>
-      <c r="M12" s="119"/>
-      <c r="N12" s="117"/>
+      <c r="K12" s="120"/>
+      <c r="L12" s="120"/>
+      <c r="M12" s="120"/>
+      <c r="N12" s="118"/>
     </row>
     <row r="13" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A13" s="110" t="s">
+      <c r="A13" s="111" t="s">
         <v>530</v>
       </c>
-      <c r="B13" s="115" t="n">
+      <c r="B13" s="116" t="n">
         <v>65535</v>
       </c>
-      <c r="C13" s="110" t="s">
+      <c r="C13" s="111" t="s">
         <v>531</v>
       </c>
-      <c r="D13" s="116"/>
-      <c r="E13" s="116"/>
-      <c r="F13" s="116"/>
-      <c r="G13" s="116"/>
-      <c r="H13" s="116"/>
-      <c r="I13" s="115" t="n">
+      <c r="D13" s="117"/>
+      <c r="E13" s="117"/>
+      <c r="F13" s="117"/>
+      <c r="G13" s="117"/>
+      <c r="H13" s="117"/>
+      <c r="I13" s="116" t="n">
         <v>50</v>
       </c>
-      <c r="J13" s="115" t="n">
+      <c r="J13" s="116" t="n">
         <v>65</v>
       </c>
-      <c r="K13" s="116"/>
-      <c r="L13" s="116"/>
-      <c r="M13" s="116"/>
-      <c r="N13" s="110"/>
+      <c r="K13" s="117"/>
+      <c r="L13" s="117"/>
+      <c r="M13" s="117"/>
+      <c r="N13" s="111"/>
     </row>
     <row r="14" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A14" s="117" t="s">
+      <c r="A14" s="118" t="s">
         <v>532</v>
       </c>
-      <c r="B14" s="118" t="n">
+      <c r="B14" s="119" t="n">
         <v>180</v>
       </c>
-      <c r="C14" s="117" t="s">
+      <c r="C14" s="118" t="s">
         <v>527</v>
       </c>
-      <c r="D14" s="119"/>
-      <c r="E14" s="119"/>
-      <c r="F14" s="119"/>
-      <c r="G14" s="119"/>
-      <c r="H14" s="119"/>
-      <c r="I14" s="118" t="n">
+      <c r="D14" s="120"/>
+      <c r="E14" s="120"/>
+      <c r="F14" s="120"/>
+      <c r="G14" s="120"/>
+      <c r="H14" s="120"/>
+      <c r="I14" s="119" t="n">
         <v>280</v>
       </c>
-      <c r="J14" s="118" t="n">
+      <c r="J14" s="119" t="n">
         <v>330</v>
       </c>
-      <c r="K14" s="119"/>
-      <c r="L14" s="119"/>
-      <c r="M14" s="119"/>
-      <c r="N14" s="117"/>
+      <c r="K14" s="120"/>
+      <c r="L14" s="120"/>
+      <c r="M14" s="120"/>
+      <c r="N14" s="118"/>
     </row>
     <row r="15" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A15" s="110" t="s">
+      <c r="A15" s="111" t="s">
         <v>532</v>
       </c>
-      <c r="B15" s="115" t="n">
+      <c r="B15" s="116" t="n">
         <v>365</v>
       </c>
-      <c r="C15" s="110" t="s">
+      <c r="C15" s="111" t="s">
         <v>528</v>
       </c>
-      <c r="D15" s="116"/>
-      <c r="E15" s="116"/>
-      <c r="F15" s="116"/>
-      <c r="G15" s="116"/>
-      <c r="H15" s="116"/>
-      <c r="I15" s="115" t="n">
+      <c r="D15" s="117"/>
+      <c r="E15" s="117"/>
+      <c r="F15" s="117"/>
+      <c r="G15" s="117"/>
+      <c r="H15" s="117"/>
+      <c r="I15" s="116" t="n">
         <v>180</v>
       </c>
-      <c r="J15" s="115" t="n">
+      <c r="J15" s="116" t="n">
         <v>210</v>
       </c>
-      <c r="K15" s="116"/>
-      <c r="L15" s="116"/>
-      <c r="M15" s="116"/>
-      <c r="N15" s="110"/>
+      <c r="K15" s="117"/>
+      <c r="L15" s="117"/>
+      <c r="M15" s="117"/>
+      <c r="N15" s="111"/>
     </row>
     <row r="16" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A16" s="117" t="s">
+      <c r="A16" s="118" t="s">
         <v>532</v>
       </c>
-      <c r="B16" s="118" t="n">
+      <c r="B16" s="119" t="n">
         <v>1460</v>
       </c>
-      <c r="C16" s="117" t="s">
+      <c r="C16" s="118" t="s">
         <v>529</v>
       </c>
-      <c r="D16" s="119"/>
-      <c r="E16" s="119"/>
-      <c r="F16" s="119"/>
-      <c r="G16" s="119"/>
-      <c r="H16" s="119"/>
-      <c r="I16" s="118" t="n">
+      <c r="D16" s="120"/>
+      <c r="E16" s="120"/>
+      <c r="F16" s="120"/>
+      <c r="G16" s="120"/>
+      <c r="H16" s="120"/>
+      <c r="I16" s="119" t="n">
         <v>75</v>
       </c>
-      <c r="J16" s="118" t="n">
+      <c r="J16" s="119" t="n">
         <v>90</v>
       </c>
-      <c r="K16" s="119"/>
-      <c r="L16" s="119"/>
-      <c r="M16" s="119"/>
-      <c r="N16" s="117"/>
+      <c r="K16" s="120"/>
+      <c r="L16" s="120"/>
+      <c r="M16" s="120"/>
+      <c r="N16" s="118"/>
     </row>
     <row r="17" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A17" s="110" t="s">
+      <c r="A17" s="111" t="s">
         <v>530</v>
       </c>
-      <c r="B17" s="115" t="n">
+      <c r="B17" s="116" t="n">
         <v>4380</v>
       </c>
-      <c r="C17" s="110" t="s">
+      <c r="C17" s="111" t="s">
         <v>531</v>
       </c>
-      <c r="D17" s="116"/>
-      <c r="E17" s="116"/>
-      <c r="F17" s="116"/>
-      <c r="G17" s="116"/>
-      <c r="H17" s="116"/>
-      <c r="I17" s="115" t="n">
+      <c r="D17" s="117"/>
+      <c r="E17" s="117"/>
+      <c r="F17" s="117"/>
+      <c r="G17" s="117"/>
+      <c r="H17" s="117"/>
+      <c r="I17" s="116" t="n">
         <v>50</v>
       </c>
-      <c r="J17" s="116"/>
-      <c r="K17" s="116"/>
-      <c r="L17" s="116"/>
-      <c r="M17" s="116"/>
-      <c r="N17" s="110"/>
+      <c r="J17" s="117"/>
+      <c r="K17" s="117"/>
+      <c r="L17" s="117"/>
+      <c r="M17" s="117"/>
+      <c r="N17" s="111"/>
     </row>
     <row r="18" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A18" s="117" t="s">
+      <c r="A18" s="118" t="s">
         <v>526</v>
       </c>
-      <c r="B18" s="118" t="n">
+      <c r="B18" s="119" t="n">
         <v>4380</v>
       </c>
-      <c r="C18" s="117" t="s">
+      <c r="C18" s="118" t="s">
         <v>531</v>
       </c>
-      <c r="D18" s="119"/>
-      <c r="E18" s="119"/>
-      <c r="F18" s="119"/>
-      <c r="G18" s="119"/>
-      <c r="H18" s="119"/>
-      <c r="I18" s="118" t="n">
+      <c r="D18" s="120"/>
+      <c r="E18" s="120"/>
+      <c r="F18" s="120"/>
+      <c r="G18" s="120"/>
+      <c r="H18" s="120"/>
+      <c r="I18" s="119" t="n">
         <v>50</v>
       </c>
-      <c r="J18" s="119"/>
-      <c r="K18" s="119"/>
-      <c r="L18" s="119"/>
-      <c r="M18" s="119"/>
-      <c r="N18" s="117"/>
+      <c r="J18" s="120"/>
+      <c r="K18" s="120"/>
+      <c r="L18" s="120"/>
+      <c r="M18" s="120"/>
+      <c r="N18" s="118"/>
     </row>
     <row r="19" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A19" s="110" t="s">
+      <c r="A19" s="111" t="s">
         <v>532</v>
       </c>
-      <c r="B19" s="115" t="n">
+      <c r="B19" s="116" t="n">
         <v>4380</v>
       </c>
-      <c r="C19" s="110" t="s">
+      <c r="C19" s="111" t="s">
         <v>531</v>
       </c>
-      <c r="D19" s="116"/>
-      <c r="E19" s="116"/>
-      <c r="F19" s="116"/>
-      <c r="G19" s="116"/>
-      <c r="H19" s="116"/>
-      <c r="I19" s="115" t="n">
+      <c r="D19" s="117"/>
+      <c r="E19" s="117"/>
+      <c r="F19" s="117"/>
+      <c r="G19" s="117"/>
+      <c r="H19" s="117"/>
+      <c r="I19" s="116" t="n">
         <v>50</v>
       </c>
-      <c r="J19" s="116"/>
-      <c r="K19" s="116"/>
-      <c r="L19" s="116"/>
-      <c r="M19" s="116"/>
-      <c r="N19" s="110"/>
+      <c r="J19" s="117"/>
+      <c r="K19" s="117"/>
+      <c r="L19" s="117"/>
+      <c r="M19" s="117"/>
+      <c r="N19" s="111"/>
     </row>
     <row r="22" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">

</xml_diff>

<commit_message>
Added three new markers, tested on sample of Daniell-Zak-101092126300.csv file. CITROBACSEQA712, PSEUDOMSEQA712 are present in mentioned file while PROVSEQ712A is not, so it is not tested, but it should work.
</commit_message>
<xml_diff>
--- a/HealthPath/CreatingReport/Matrix.xlsx
+++ b/HealthPath/CreatingReport/Matrix.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="776" uniqueCount="536">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="794" uniqueCount="543">
   <si>
     <t xml:space="preserve">Code</t>
   </si>
@@ -2025,6 +2025,27 @@
     <t xml:space="preserve">Low levels of Beta-glucurondiase are not associated with any negative outcome.</t>
   </si>
   <si>
+    <t xml:space="preserve">CITROBACSEQA712</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Citrobacter spp.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PSEUDOMSEQA712</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pseudomonas spp.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt; 5,0 x 10^7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PROVSEQ712A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Providencia spp.</t>
+  </si>
+  <si>
     <t xml:space="preserve">14 von 14 Datensätze werden angezeigt.</t>
   </si>
   <si>
@@ -2109,7 +2130,7 @@
     <numFmt numFmtId="165" formatCode="@"/>
     <numFmt numFmtId="166" formatCode="0"/>
   </numFmts>
-  <fonts count="27">
+  <fonts count="28">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -2286,6 +2307,13 @@
       <color rgb="FF0070C0"/>
       <name val="Avenir Book"/>
       <family val="0"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <charset val="1"/>
     </font>
     <font>
@@ -2488,7 +2516,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="121">
+  <cellXfs count="127">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -2929,47 +2957,71 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="25" fillId="10" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="15" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="7" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="15" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="26" fillId="10" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="25" fillId="8" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="26" fillId="8" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="25" fillId="10" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="26" fillId="10" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="26" fillId="11" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="27" fillId="11" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="26" fillId="11" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="27" fillId="11" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="26" fillId="11" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="27" fillId="11" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="25" fillId="8" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="26" fillId="8" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="25" fillId="8" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="26" fillId="8" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="25" fillId="12" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="26" fillId="12" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="25" fillId="12" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="26" fillId="12" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="25" fillId="12" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="26" fillId="12" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -3052,8 +3104,8 @@
   </sheetPr>
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D174" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F194" activeCellId="0" sqref="F194"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A279" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F290" activeCellId="0" sqref="F290"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -9455,102 +9507,168 @@
       <c r="M303" s="12"/>
     </row>
     <row r="304" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="E304" s="12"/>
-      <c r="F304" s="12"/>
-      <c r="G304" s="12"/>
-      <c r="H304" s="12"/>
-      <c r="I304" s="12"/>
-      <c r="J304" s="12"/>
-      <c r="K304" s="12"/>
-      <c r="L304" s="12"/>
+      <c r="A304" s="110" t="s">
+        <v>511</v>
+      </c>
+      <c r="B304" s="111" t="s">
+        <v>512</v>
+      </c>
+      <c r="C304" s="28"/>
+      <c r="D304" s="112"/>
+      <c r="E304" s="113"/>
+      <c r="F304" s="113"/>
+      <c r="G304" s="113"/>
+      <c r="H304" s="113" t="s">
+        <v>293</v>
+      </c>
+      <c r="I304" s="113" t="s">
+        <v>109</v>
+      </c>
+      <c r="J304" s="113" t="s">
+        <v>180</v>
+      </c>
+      <c r="K304" s="113" t="s">
+        <v>182</v>
+      </c>
+      <c r="L304" s="113"/>
       <c r="M304" s="12"/>
     </row>
     <row r="305" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="E305" s="12"/>
-      <c r="F305" s="12"/>
-      <c r="G305" s="12"/>
-      <c r="H305" s="12"/>
-      <c r="I305" s="12"/>
-      <c r="J305" s="12"/>
-      <c r="K305" s="12"/>
-      <c r="L305" s="12"/>
+      <c r="B305" s="114"/>
+      <c r="C305" s="28"/>
+      <c r="D305" s="112"/>
+      <c r="E305" s="113"/>
+      <c r="F305" s="113"/>
+      <c r="G305" s="113"/>
+      <c r="H305" s="113"/>
+      <c r="I305" s="113"/>
+      <c r="J305" s="113"/>
+      <c r="K305" s="113"/>
+      <c r="L305" s="113"/>
       <c r="M305" s="12"/>
     </row>
     <row r="306" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="E306" s="12"/>
-      <c r="F306" s="12"/>
-      <c r="G306" s="12"/>
-      <c r="H306" s="12"/>
-      <c r="I306" s="12"/>
-      <c r="J306" s="12"/>
-      <c r="K306" s="12"/>
-      <c r="L306" s="12"/>
+      <c r="B306" s="115"/>
+      <c r="C306" s="90"/>
+      <c r="D306" s="112"/>
+      <c r="E306" s="113"/>
+      <c r="F306" s="113"/>
+      <c r="G306" s="113"/>
+      <c r="H306" s="113"/>
+      <c r="I306" s="113"/>
+      <c r="J306" s="113"/>
+      <c r="K306" s="113"/>
+      <c r="L306" s="113"/>
       <c r="M306" s="12"/>
     </row>
     <row r="307" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="E307" s="12"/>
-      <c r="F307" s="12"/>
-      <c r="G307" s="12"/>
-      <c r="H307" s="12"/>
-      <c r="I307" s="12"/>
-      <c r="J307" s="12"/>
-      <c r="K307" s="12"/>
-      <c r="L307" s="12"/>
+      <c r="A307" s="110" t="s">
+        <v>513</v>
+      </c>
+      <c r="B307" s="111" t="s">
+        <v>514</v>
+      </c>
+      <c r="C307" s="28"/>
+      <c r="D307" s="112"/>
+      <c r="E307" s="113"/>
+      <c r="F307" s="113"/>
+      <c r="G307" s="113"/>
+      <c r="H307" s="113" t="s">
+        <v>515</v>
+      </c>
+      <c r="I307" s="113" t="s">
+        <v>142</v>
+      </c>
+      <c r="J307" s="113" t="s">
+        <v>109</v>
+      </c>
+      <c r="K307" s="113" t="s">
+        <v>180</v>
+      </c>
+      <c r="L307" s="113"/>
       <c r="M307" s="12"/>
     </row>
     <row r="308" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="E308" s="12"/>
-      <c r="F308" s="12"/>
-      <c r="G308" s="12"/>
-      <c r="H308" s="12"/>
-      <c r="I308" s="12"/>
-      <c r="J308" s="12"/>
-      <c r="K308" s="12"/>
-      <c r="L308" s="12"/>
+      <c r="B308" s="114"/>
+      <c r="C308" s="28"/>
+      <c r="D308" s="112"/>
+      <c r="E308" s="113"/>
+      <c r="F308" s="113"/>
+      <c r="G308" s="113"/>
+      <c r="H308" s="113"/>
+      <c r="I308" s="113"/>
+      <c r="J308" s="113"/>
+      <c r="K308" s="113"/>
+      <c r="L308" s="113"/>
       <c r="M308" s="12"/>
     </row>
     <row r="309" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="E309" s="12"/>
-      <c r="F309" s="12"/>
-      <c r="G309" s="12"/>
-      <c r="H309" s="12"/>
-      <c r="I309" s="12"/>
-      <c r="J309" s="12"/>
-      <c r="K309" s="12"/>
-      <c r="L309" s="12"/>
+      <c r="B309" s="115"/>
+      <c r="C309" s="90"/>
+      <c r="D309" s="112"/>
+      <c r="E309" s="113"/>
+      <c r="F309" s="113"/>
+      <c r="G309" s="113"/>
+      <c r="H309" s="113"/>
+      <c r="I309" s="113"/>
+      <c r="J309" s="113"/>
+      <c r="K309" s="113"/>
+      <c r="L309" s="113"/>
       <c r="M309" s="12"/>
     </row>
     <row r="310" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="E310" s="12"/>
-      <c r="F310" s="12"/>
-      <c r="G310" s="12"/>
-      <c r="H310" s="12"/>
-      <c r="I310" s="12"/>
-      <c r="J310" s="12"/>
-      <c r="K310" s="12"/>
-      <c r="L310" s="12"/>
+      <c r="A310" s="110" t="s">
+        <v>516</v>
+      </c>
+      <c r="B310" s="111" t="s">
+        <v>517</v>
+      </c>
+      <c r="C310" s="28"/>
+      <c r="D310" s="112"/>
+      <c r="E310" s="113"/>
+      <c r="F310" s="113"/>
+      <c r="G310" s="113"/>
+      <c r="H310" s="113" t="s">
+        <v>515</v>
+      </c>
+      <c r="I310" s="113" t="s">
+        <v>142</v>
+      </c>
+      <c r="J310" s="113" t="s">
+        <v>109</v>
+      </c>
+      <c r="K310" s="113" t="s">
+        <v>180</v>
+      </c>
+      <c r="L310" s="113"/>
       <c r="M310" s="12"/>
     </row>
     <row r="311" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="E311" s="12"/>
-      <c r="F311" s="12"/>
-      <c r="G311" s="12"/>
-      <c r="H311" s="12"/>
-      <c r="I311" s="12"/>
-      <c r="J311" s="12"/>
-      <c r="K311" s="12"/>
-      <c r="L311" s="12"/>
+      <c r="B311" s="114"/>
+      <c r="C311" s="28"/>
+      <c r="D311" s="112"/>
+      <c r="E311" s="113"/>
+      <c r="F311" s="113"/>
+      <c r="G311" s="113"/>
+      <c r="H311" s="113"/>
+      <c r="I311" s="113"/>
+      <c r="J311" s="113"/>
+      <c r="K311" s="113"/>
+      <c r="L311" s="113"/>
       <c r="M311" s="12"/>
     </row>
     <row r="312" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="E312" s="12"/>
-      <c r="F312" s="12"/>
-      <c r="G312" s="12"/>
-      <c r="H312" s="12"/>
-      <c r="I312" s="12"/>
-      <c r="J312" s="12"/>
-      <c r="K312" s="12"/>
-      <c r="L312" s="12"/>
+      <c r="B312" s="115"/>
+      <c r="C312" s="90"/>
+      <c r="D312" s="112"/>
+      <c r="E312" s="113"/>
+      <c r="F312" s="113"/>
+      <c r="G312" s="113"/>
+      <c r="H312" s="113"/>
+      <c r="I312" s="113"/>
+      <c r="J312" s="113"/>
+      <c r="K312" s="113"/>
+      <c r="L312" s="113"/>
       <c r="M312" s="12"/>
     </row>
     <row r="313" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -17122,7 +17240,7 @@
       <c r="M1000" s="12"/>
     </row>
   </sheetData>
-  <mergeCells count="85">
+  <mergeCells count="88">
     <mergeCell ref="B2:D2"/>
     <mergeCell ref="B6:D6"/>
     <mergeCell ref="B9:D9"/>
@@ -17208,6 +17326,9 @@
     <mergeCell ref="D286:D288"/>
     <mergeCell ref="C295:C297"/>
     <mergeCell ref="D298:D300"/>
+    <mergeCell ref="D304:D306"/>
+    <mergeCell ref="D307:D309"/>
+    <mergeCell ref="D310:D312"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
@@ -17226,7 +17347,7 @@
   </sheetPr>
   <dimension ref="A1:N1000"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -17245,438 +17366,438 @@
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="110" t="s">
-        <v>511</v>
-      </c>
-      <c r="B4" s="111"/>
-      <c r="C4" s="111"/>
-      <c r="D4" s="111"/>
-      <c r="E4" s="111"/>
-      <c r="F4" s="111"/>
-      <c r="G4" s="111"/>
-      <c r="H4" s="111"/>
-      <c r="I4" s="111"/>
-      <c r="J4" s="111"/>
-      <c r="K4" s="111"/>
-      <c r="L4" s="111"/>
-      <c r="M4" s="111"/>
-      <c r="N4" s="111"/>
+      <c r="A4" s="116" t="s">
+        <v>518</v>
+      </c>
+      <c r="B4" s="117"/>
+      <c r="C4" s="117"/>
+      <c r="D4" s="117"/>
+      <c r="E4" s="117"/>
+      <c r="F4" s="117"/>
+      <c r="G4" s="117"/>
+      <c r="H4" s="117"/>
+      <c r="I4" s="117"/>
+      <c r="J4" s="117"/>
+      <c r="K4" s="117"/>
+      <c r="L4" s="117"/>
+      <c r="M4" s="117"/>
+      <c r="N4" s="117"/>
     </row>
     <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="110" t="s">
-        <v>512</v>
-      </c>
-      <c r="B5" s="112" t="s">
-        <v>513</v>
-      </c>
-      <c r="C5" s="110" t="s">
-        <v>514</v>
-      </c>
-      <c r="D5" s="112" t="s">
-        <v>515</v>
-      </c>
-      <c r="E5" s="112" t="s">
-        <v>516</v>
-      </c>
-      <c r="F5" s="112" t="s">
-        <v>517</v>
-      </c>
-      <c r="G5" s="112" t="s">
-        <v>518</v>
-      </c>
-      <c r="H5" s="112" t="s">
+      <c r="A5" s="116" t="s">
         <v>519</v>
       </c>
-      <c r="I5" s="112" t="s">
+      <c r="B5" s="118" t="s">
         <v>520</v>
       </c>
-      <c r="J5" s="112" t="s">
+      <c r="C5" s="116" t="s">
         <v>521</v>
       </c>
-      <c r="K5" s="112" t="s">
+      <c r="D5" s="118" t="s">
         <v>522</v>
       </c>
-      <c r="L5" s="112" t="s">
+      <c r="E5" s="118" t="s">
         <v>523</v>
       </c>
-      <c r="M5" s="112" t="s">
+      <c r="F5" s="118" t="s">
         <v>524</v>
       </c>
-      <c r="N5" s="110" t="s">
+      <c r="G5" s="118" t="s">
         <v>525</v>
       </c>
+      <c r="H5" s="118" t="s">
+        <v>526</v>
+      </c>
+      <c r="I5" s="118" t="s">
+        <v>527</v>
+      </c>
+      <c r="J5" s="118" t="s">
+        <v>528</v>
+      </c>
+      <c r="K5" s="118" t="s">
+        <v>529</v>
+      </c>
+      <c r="L5" s="118" t="s">
+        <v>530</v>
+      </c>
+      <c r="M5" s="118" t="s">
+        <v>531</v>
+      </c>
+      <c r="N5" s="116" t="s">
+        <v>532</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="113" t="s">
-        <v>526</v>
-      </c>
-      <c r="B6" s="114" t="n">
+      <c r="A6" s="119" t="s">
+        <v>533</v>
+      </c>
+      <c r="B6" s="120" t="n">
         <v>180</v>
       </c>
-      <c r="C6" s="113" t="s">
-        <v>527</v>
-      </c>
-      <c r="D6" s="115"/>
-      <c r="E6" s="115"/>
-      <c r="F6" s="115"/>
-      <c r="G6" s="115"/>
-      <c r="H6" s="115"/>
-      <c r="I6" s="114" t="n">
+      <c r="C6" s="119" t="s">
+        <v>534</v>
+      </c>
+      <c r="D6" s="121"/>
+      <c r="E6" s="121"/>
+      <c r="F6" s="121"/>
+      <c r="G6" s="121"/>
+      <c r="H6" s="121"/>
+      <c r="I6" s="120" t="n">
         <v>280</v>
       </c>
-      <c r="J6" s="114" t="n">
+      <c r="J6" s="120" t="n">
         <v>330</v>
       </c>
-      <c r="K6" s="115"/>
-      <c r="L6" s="115"/>
-      <c r="M6" s="115"/>
-      <c r="N6" s="113"/>
+      <c r="K6" s="121"/>
+      <c r="L6" s="121"/>
+      <c r="M6" s="121"/>
+      <c r="N6" s="119"/>
     </row>
     <row r="7" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="111" t="s">
-        <v>526</v>
-      </c>
-      <c r="B7" s="116" t="n">
+      <c r="A7" s="117" t="s">
+        <v>533</v>
+      </c>
+      <c r="B7" s="122" t="n">
         <v>365</v>
       </c>
-      <c r="C7" s="111" t="s">
-        <v>528</v>
-      </c>
-      <c r="D7" s="117"/>
-      <c r="E7" s="117"/>
-      <c r="F7" s="117"/>
-      <c r="G7" s="117"/>
-      <c r="H7" s="117"/>
-      <c r="I7" s="116" t="n">
+      <c r="C7" s="117" t="s">
+        <v>535</v>
+      </c>
+      <c r="D7" s="123"/>
+      <c r="E7" s="123"/>
+      <c r="F7" s="123"/>
+      <c r="G7" s="123"/>
+      <c r="H7" s="123"/>
+      <c r="I7" s="122" t="n">
         <v>180</v>
       </c>
-      <c r="J7" s="116" t="n">
+      <c r="J7" s="122" t="n">
         <v>210</v>
       </c>
-      <c r="K7" s="117"/>
-      <c r="L7" s="117"/>
-      <c r="M7" s="117"/>
-      <c r="N7" s="111"/>
+      <c r="K7" s="123"/>
+      <c r="L7" s="123"/>
+      <c r="M7" s="123"/>
+      <c r="N7" s="117"/>
     </row>
     <row r="8" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="118" t="s">
-        <v>526</v>
-      </c>
-      <c r="B8" s="119" t="n">
+      <c r="A8" s="124" t="s">
+        <v>533</v>
+      </c>
+      <c r="B8" s="125" t="n">
         <v>1460</v>
       </c>
-      <c r="C8" s="118" t="s">
-        <v>529</v>
-      </c>
-      <c r="D8" s="120"/>
-      <c r="E8" s="120"/>
-      <c r="F8" s="120"/>
-      <c r="G8" s="120"/>
-      <c r="H8" s="120"/>
-      <c r="I8" s="119" t="n">
+      <c r="C8" s="124" t="s">
+        <v>536</v>
+      </c>
+      <c r="D8" s="126"/>
+      <c r="E8" s="126"/>
+      <c r="F8" s="126"/>
+      <c r="G8" s="126"/>
+      <c r="H8" s="126"/>
+      <c r="I8" s="125" t="n">
         <v>75</v>
       </c>
-      <c r="J8" s="119" t="n">
+      <c r="J8" s="125" t="n">
         <v>90</v>
       </c>
-      <c r="K8" s="120"/>
-      <c r="L8" s="120"/>
-      <c r="M8" s="120"/>
-      <c r="N8" s="118"/>
+      <c r="K8" s="126"/>
+      <c r="L8" s="126"/>
+      <c r="M8" s="126"/>
+      <c r="N8" s="124"/>
     </row>
     <row r="9" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="111" t="s">
-        <v>530</v>
-      </c>
-      <c r="B9" s="116" t="n">
+      <c r="A9" s="117" t="s">
+        <v>537</v>
+      </c>
+      <c r="B9" s="122" t="n">
         <v>180</v>
       </c>
-      <c r="C9" s="111" t="s">
-        <v>527</v>
-      </c>
-      <c r="D9" s="117"/>
-      <c r="E9" s="117"/>
-      <c r="F9" s="117"/>
-      <c r="G9" s="117"/>
-      <c r="H9" s="117"/>
-      <c r="I9" s="116" t="n">
+      <c r="C9" s="117" t="s">
+        <v>534</v>
+      </c>
+      <c r="D9" s="123"/>
+      <c r="E9" s="123"/>
+      <c r="F9" s="123"/>
+      <c r="G9" s="123"/>
+      <c r="H9" s="123"/>
+      <c r="I9" s="122" t="n">
         <v>280</v>
       </c>
-      <c r="J9" s="116" t="n">
+      <c r="J9" s="122" t="n">
         <v>330</v>
       </c>
-      <c r="K9" s="117"/>
-      <c r="L9" s="117"/>
-      <c r="M9" s="117"/>
-      <c r="N9" s="111"/>
+      <c r="K9" s="123"/>
+      <c r="L9" s="123"/>
+      <c r="M9" s="123"/>
+      <c r="N9" s="117"/>
     </row>
     <row r="10" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="118" t="s">
-        <v>530</v>
-      </c>
-      <c r="B10" s="119" t="n">
+      <c r="A10" s="124" t="s">
+        <v>537</v>
+      </c>
+      <c r="B10" s="125" t="n">
         <v>365</v>
       </c>
-      <c r="C10" s="118" t="s">
-        <v>528</v>
-      </c>
-      <c r="D10" s="120"/>
-      <c r="E10" s="120"/>
-      <c r="F10" s="120"/>
-      <c r="G10" s="120"/>
-      <c r="H10" s="120"/>
-      <c r="I10" s="119" t="n">
+      <c r="C10" s="124" t="s">
+        <v>535</v>
+      </c>
+      <c r="D10" s="126"/>
+      <c r="E10" s="126"/>
+      <c r="F10" s="126"/>
+      <c r="G10" s="126"/>
+      <c r="H10" s="126"/>
+      <c r="I10" s="125" t="n">
         <v>180</v>
       </c>
-      <c r="J10" s="119" t="n">
+      <c r="J10" s="125" t="n">
         <v>210</v>
       </c>
-      <c r="K10" s="120"/>
-      <c r="L10" s="120"/>
-      <c r="M10" s="120"/>
-      <c r="N10" s="118"/>
+      <c r="K10" s="126"/>
+      <c r="L10" s="126"/>
+      <c r="M10" s="126"/>
+      <c r="N10" s="124"/>
     </row>
     <row r="11" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A11" s="111" t="s">
-        <v>530</v>
-      </c>
-      <c r="B11" s="116" t="n">
+      <c r="A11" s="117" t="s">
+        <v>537</v>
+      </c>
+      <c r="B11" s="122" t="n">
         <v>1460</v>
       </c>
-      <c r="C11" s="111" t="s">
-        <v>529</v>
-      </c>
-      <c r="D11" s="117"/>
-      <c r="E11" s="117"/>
-      <c r="F11" s="117"/>
-      <c r="G11" s="117"/>
-      <c r="H11" s="117"/>
-      <c r="I11" s="116" t="n">
+      <c r="C11" s="117" t="s">
+        <v>536</v>
+      </c>
+      <c r="D11" s="123"/>
+      <c r="E11" s="123"/>
+      <c r="F11" s="123"/>
+      <c r="G11" s="123"/>
+      <c r="H11" s="123"/>
+      <c r="I11" s="122" t="n">
         <v>75</v>
       </c>
-      <c r="J11" s="116" t="n">
+      <c r="J11" s="122" t="n">
         <v>90</v>
       </c>
-      <c r="K11" s="117"/>
-      <c r="L11" s="117"/>
-      <c r="M11" s="117"/>
-      <c r="N11" s="111"/>
+      <c r="K11" s="123"/>
+      <c r="L11" s="123"/>
+      <c r="M11" s="123"/>
+      <c r="N11" s="117"/>
     </row>
     <row r="12" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A12" s="118" t="s">
-        <v>526</v>
-      </c>
-      <c r="B12" s="119" t="n">
+      <c r="A12" s="124" t="s">
+        <v>533</v>
+      </c>
+      <c r="B12" s="125" t="n">
         <v>65535</v>
       </c>
-      <c r="C12" s="118" t="s">
-        <v>531</v>
-      </c>
-      <c r="D12" s="120"/>
-      <c r="E12" s="120"/>
-      <c r="F12" s="120"/>
-      <c r="G12" s="120"/>
-      <c r="H12" s="120"/>
-      <c r="I12" s="119" t="n">
+      <c r="C12" s="124" t="s">
+        <v>538</v>
+      </c>
+      <c r="D12" s="126"/>
+      <c r="E12" s="126"/>
+      <c r="F12" s="126"/>
+      <c r="G12" s="126"/>
+      <c r="H12" s="126"/>
+      <c r="I12" s="125" t="n">
         <v>50</v>
       </c>
-      <c r="J12" s="119" t="n">
+      <c r="J12" s="125" t="n">
         <v>65</v>
       </c>
-      <c r="K12" s="120"/>
-      <c r="L12" s="120"/>
-      <c r="M12" s="120"/>
-      <c r="N12" s="118"/>
+      <c r="K12" s="126"/>
+      <c r="L12" s="126"/>
+      <c r="M12" s="126"/>
+      <c r="N12" s="124"/>
     </row>
     <row r="13" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A13" s="111" t="s">
-        <v>530</v>
-      </c>
-      <c r="B13" s="116" t="n">
+      <c r="A13" s="117" t="s">
+        <v>537</v>
+      </c>
+      <c r="B13" s="122" t="n">
         <v>65535</v>
       </c>
-      <c r="C13" s="111" t="s">
-        <v>531</v>
-      </c>
-      <c r="D13" s="117"/>
-      <c r="E13" s="117"/>
-      <c r="F13" s="117"/>
-      <c r="G13" s="117"/>
-      <c r="H13" s="117"/>
-      <c r="I13" s="116" t="n">
+      <c r="C13" s="117" t="s">
+        <v>538</v>
+      </c>
+      <c r="D13" s="123"/>
+      <c r="E13" s="123"/>
+      <c r="F13" s="123"/>
+      <c r="G13" s="123"/>
+      <c r="H13" s="123"/>
+      <c r="I13" s="122" t="n">
         <v>50</v>
       </c>
-      <c r="J13" s="116" t="n">
+      <c r="J13" s="122" t="n">
         <v>65</v>
       </c>
-      <c r="K13" s="117"/>
-      <c r="L13" s="117"/>
-      <c r="M13" s="117"/>
-      <c r="N13" s="111"/>
+      <c r="K13" s="123"/>
+      <c r="L13" s="123"/>
+      <c r="M13" s="123"/>
+      <c r="N13" s="117"/>
     </row>
     <row r="14" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A14" s="118" t="s">
-        <v>532</v>
-      </c>
-      <c r="B14" s="119" t="n">
+      <c r="A14" s="124" t="s">
+        <v>539</v>
+      </c>
+      <c r="B14" s="125" t="n">
         <v>180</v>
       </c>
-      <c r="C14" s="118" t="s">
-        <v>527</v>
-      </c>
-      <c r="D14" s="120"/>
-      <c r="E14" s="120"/>
-      <c r="F14" s="120"/>
-      <c r="G14" s="120"/>
-      <c r="H14" s="120"/>
-      <c r="I14" s="119" t="n">
+      <c r="C14" s="124" t="s">
+        <v>534</v>
+      </c>
+      <c r="D14" s="126"/>
+      <c r="E14" s="126"/>
+      <c r="F14" s="126"/>
+      <c r="G14" s="126"/>
+      <c r="H14" s="126"/>
+      <c r="I14" s="125" t="n">
         <v>280</v>
       </c>
-      <c r="J14" s="119" t="n">
+      <c r="J14" s="125" t="n">
         <v>330</v>
       </c>
-      <c r="K14" s="120"/>
-      <c r="L14" s="120"/>
-      <c r="M14" s="120"/>
-      <c r="N14" s="118"/>
+      <c r="K14" s="126"/>
+      <c r="L14" s="126"/>
+      <c r="M14" s="126"/>
+      <c r="N14" s="124"/>
     </row>
     <row r="15" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A15" s="111" t="s">
-        <v>532</v>
-      </c>
-      <c r="B15" s="116" t="n">
+      <c r="A15" s="117" t="s">
+        <v>539</v>
+      </c>
+      <c r="B15" s="122" t="n">
         <v>365</v>
       </c>
-      <c r="C15" s="111" t="s">
-        <v>528</v>
-      </c>
-      <c r="D15" s="117"/>
-      <c r="E15" s="117"/>
-      <c r="F15" s="117"/>
-      <c r="G15" s="117"/>
-      <c r="H15" s="117"/>
-      <c r="I15" s="116" t="n">
+      <c r="C15" s="117" t="s">
+        <v>535</v>
+      </c>
+      <c r="D15" s="123"/>
+      <c r="E15" s="123"/>
+      <c r="F15" s="123"/>
+      <c r="G15" s="123"/>
+      <c r="H15" s="123"/>
+      <c r="I15" s="122" t="n">
         <v>180</v>
       </c>
-      <c r="J15" s="116" t="n">
+      <c r="J15" s="122" t="n">
         <v>210</v>
       </c>
-      <c r="K15" s="117"/>
-      <c r="L15" s="117"/>
-      <c r="M15" s="117"/>
-      <c r="N15" s="111"/>
+      <c r="K15" s="123"/>
+      <c r="L15" s="123"/>
+      <c r="M15" s="123"/>
+      <c r="N15" s="117"/>
     </row>
     <row r="16" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A16" s="118" t="s">
-        <v>532</v>
-      </c>
-      <c r="B16" s="119" t="n">
+      <c r="A16" s="124" t="s">
+        <v>539</v>
+      </c>
+      <c r="B16" s="125" t="n">
         <v>1460</v>
       </c>
-      <c r="C16" s="118" t="s">
-        <v>529</v>
-      </c>
-      <c r="D16" s="120"/>
-      <c r="E16" s="120"/>
-      <c r="F16" s="120"/>
-      <c r="G16" s="120"/>
-      <c r="H16" s="120"/>
-      <c r="I16" s="119" t="n">
+      <c r="C16" s="124" t="s">
+        <v>536</v>
+      </c>
+      <c r="D16" s="126"/>
+      <c r="E16" s="126"/>
+      <c r="F16" s="126"/>
+      <c r="G16" s="126"/>
+      <c r="H16" s="126"/>
+      <c r="I16" s="125" t="n">
         <v>75</v>
       </c>
-      <c r="J16" s="119" t="n">
+      <c r="J16" s="125" t="n">
         <v>90</v>
       </c>
-      <c r="K16" s="120"/>
-      <c r="L16" s="120"/>
-      <c r="M16" s="120"/>
-      <c r="N16" s="118"/>
+      <c r="K16" s="126"/>
+      <c r="L16" s="126"/>
+      <c r="M16" s="126"/>
+      <c r="N16" s="124"/>
     </row>
     <row r="17" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A17" s="111" t="s">
-        <v>530</v>
-      </c>
-      <c r="B17" s="116" t="n">
+      <c r="A17" s="117" t="s">
+        <v>537</v>
+      </c>
+      <c r="B17" s="122" t="n">
         <v>4380</v>
       </c>
-      <c r="C17" s="111" t="s">
-        <v>531</v>
-      </c>
-      <c r="D17" s="117"/>
-      <c r="E17" s="117"/>
-      <c r="F17" s="117"/>
-      <c r="G17" s="117"/>
-      <c r="H17" s="117"/>
-      <c r="I17" s="116" t="n">
+      <c r="C17" s="117" t="s">
+        <v>538</v>
+      </c>
+      <c r="D17" s="123"/>
+      <c r="E17" s="123"/>
+      <c r="F17" s="123"/>
+      <c r="G17" s="123"/>
+      <c r="H17" s="123"/>
+      <c r="I17" s="122" t="n">
         <v>50</v>
       </c>
-      <c r="J17" s="117"/>
-      <c r="K17" s="117"/>
-      <c r="L17" s="117"/>
-      <c r="M17" s="117"/>
-      <c r="N17" s="111"/>
+      <c r="J17" s="123"/>
+      <c r="K17" s="123"/>
+      <c r="L17" s="123"/>
+      <c r="M17" s="123"/>
+      <c r="N17" s="117"/>
     </row>
     <row r="18" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A18" s="118" t="s">
-        <v>526</v>
-      </c>
-      <c r="B18" s="119" t="n">
+      <c r="A18" s="124" t="s">
+        <v>533</v>
+      </c>
+      <c r="B18" s="125" t="n">
         <v>4380</v>
       </c>
-      <c r="C18" s="118" t="s">
-        <v>531</v>
-      </c>
-      <c r="D18" s="120"/>
-      <c r="E18" s="120"/>
-      <c r="F18" s="120"/>
-      <c r="G18" s="120"/>
-      <c r="H18" s="120"/>
-      <c r="I18" s="119" t="n">
+      <c r="C18" s="124" t="s">
+        <v>538</v>
+      </c>
+      <c r="D18" s="126"/>
+      <c r="E18" s="126"/>
+      <c r="F18" s="126"/>
+      <c r="G18" s="126"/>
+      <c r="H18" s="126"/>
+      <c r="I18" s="125" t="n">
         <v>50</v>
       </c>
-      <c r="J18" s="120"/>
-      <c r="K18" s="120"/>
-      <c r="L18" s="120"/>
-      <c r="M18" s="120"/>
-      <c r="N18" s="118"/>
+      <c r="J18" s="126"/>
+      <c r="K18" s="126"/>
+      <c r="L18" s="126"/>
+      <c r="M18" s="126"/>
+      <c r="N18" s="124"/>
     </row>
     <row r="19" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A19" s="111" t="s">
-        <v>532</v>
-      </c>
-      <c r="B19" s="116" t="n">
+      <c r="A19" s="117" t="s">
+        <v>539</v>
+      </c>
+      <c r="B19" s="122" t="n">
         <v>4380</v>
       </c>
-      <c r="C19" s="111" t="s">
-        <v>531</v>
-      </c>
-      <c r="D19" s="117"/>
-      <c r="E19" s="117"/>
-      <c r="F19" s="117"/>
-      <c r="G19" s="117"/>
-      <c r="H19" s="117"/>
-      <c r="I19" s="116" t="n">
+      <c r="C19" s="117" t="s">
+        <v>538</v>
+      </c>
+      <c r="D19" s="123"/>
+      <c r="E19" s="123"/>
+      <c r="F19" s="123"/>
+      <c r="G19" s="123"/>
+      <c r="H19" s="123"/>
+      <c r="I19" s="122" t="n">
         <v>50</v>
       </c>
-      <c r="J19" s="117"/>
-      <c r="K19" s="117"/>
-      <c r="L19" s="117"/>
-      <c r="M19" s="117"/>
-      <c r="N19" s="111"/>
+      <c r="J19" s="123"/>
+      <c r="K19" s="123"/>
+      <c r="L19" s="123"/>
+      <c r="M19" s="123"/>
+      <c r="N19" s="117"/>
     </row>
     <row r="22" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
-        <v>533</v>
+        <v>540</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="s">
-        <v>534</v>
+        <v>541</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="s">
-        <v>535</v>
+        <v>542</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>

</xml_diff>

<commit_message>
chaned PROVSEQA712A marker code
</commit_message>
<xml_diff>
--- a/HealthPath/CreatingReport/Matrix.xlsx
+++ b/HealthPath/CreatingReport/Matrix.xlsx
@@ -2040,7 +2040,7 @@
     <t xml:space="preserve">&lt; 5,0 x 10^7</t>
   </si>
   <si>
-    <t xml:space="preserve">PROVSEQ712A</t>
+    <t xml:space="preserve">PROVSEQA712A</t>
   </si>
   <si>
     <t xml:space="preserve">Providencia spp.</t>
@@ -2130,7 +2130,7 @@
     <numFmt numFmtId="165" formatCode="@"/>
     <numFmt numFmtId="166" formatCode="0"/>
   </numFmts>
-  <fonts count="28">
+  <fonts count="29">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -2315,6 +2315,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="8"/>
@@ -2516,7 +2522,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="127">
+  <cellXfs count="128">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -2981,47 +2987,51 @@
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="26" fillId="10" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="27" fillId="10" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="26" fillId="8" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="27" fillId="8" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="26" fillId="10" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="27" fillId="10" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="27" fillId="11" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="28" fillId="11" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="27" fillId="11" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="28" fillId="11" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="27" fillId="11" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="28" fillId="11" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="26" fillId="8" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="27" fillId="8" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="26" fillId="8" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="27" fillId="8" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="26" fillId="12" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="27" fillId="12" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="26" fillId="12" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="27" fillId="12" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="26" fillId="12" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="27" fillId="12" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -3105,7 +3115,7 @@
   <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A279" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F290" activeCellId="0" sqref="F290"/>
+      <selection pane="topLeft" activeCell="A310" activeCellId="0" sqref="A310"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -9617,7 +9627,7 @@
       <c r="M309" s="12"/>
     </row>
     <row r="310" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A310" s="110" t="s">
+      <c r="A310" s="116" t="s">
         <v>516</v>
       </c>
       <c r="B310" s="111" t="s">
@@ -17366,424 +17376,424 @@
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="116" t="s">
+      <c r="A4" s="117" t="s">
         <v>518</v>
       </c>
-      <c r="B4" s="117"/>
-      <c r="C4" s="117"/>
-      <c r="D4" s="117"/>
-      <c r="E4" s="117"/>
-      <c r="F4" s="117"/>
-      <c r="G4" s="117"/>
-      <c r="H4" s="117"/>
-      <c r="I4" s="117"/>
-      <c r="J4" s="117"/>
-      <c r="K4" s="117"/>
-      <c r="L4" s="117"/>
-      <c r="M4" s="117"/>
-      <c r="N4" s="117"/>
+      <c r="B4" s="118"/>
+      <c r="C4" s="118"/>
+      <c r="D4" s="118"/>
+      <c r="E4" s="118"/>
+      <c r="F4" s="118"/>
+      <c r="G4" s="118"/>
+      <c r="H4" s="118"/>
+      <c r="I4" s="118"/>
+      <c r="J4" s="118"/>
+      <c r="K4" s="118"/>
+      <c r="L4" s="118"/>
+      <c r="M4" s="118"/>
+      <c r="N4" s="118"/>
     </row>
     <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="116" t="s">
+      <c r="A5" s="117" t="s">
         <v>519</v>
       </c>
-      <c r="B5" s="118" t="s">
+      <c r="B5" s="119" t="s">
         <v>520</v>
       </c>
-      <c r="C5" s="116" t="s">
+      <c r="C5" s="117" t="s">
         <v>521</v>
       </c>
-      <c r="D5" s="118" t="s">
+      <c r="D5" s="119" t="s">
         <v>522</v>
       </c>
-      <c r="E5" s="118" t="s">
+      <c r="E5" s="119" t="s">
         <v>523</v>
       </c>
-      <c r="F5" s="118" t="s">
+      <c r="F5" s="119" t="s">
         <v>524</v>
       </c>
-      <c r="G5" s="118" t="s">
+      <c r="G5" s="119" t="s">
         <v>525</v>
       </c>
-      <c r="H5" s="118" t="s">
+      <c r="H5" s="119" t="s">
         <v>526</v>
       </c>
-      <c r="I5" s="118" t="s">
+      <c r="I5" s="119" t="s">
         <v>527</v>
       </c>
-      <c r="J5" s="118" t="s">
+      <c r="J5" s="119" t="s">
         <v>528</v>
       </c>
-      <c r="K5" s="118" t="s">
+      <c r="K5" s="119" t="s">
         <v>529</v>
       </c>
-      <c r="L5" s="118" t="s">
+      <c r="L5" s="119" t="s">
         <v>530</v>
       </c>
-      <c r="M5" s="118" t="s">
+      <c r="M5" s="119" t="s">
         <v>531</v>
       </c>
-      <c r="N5" s="116" t="s">
+      <c r="N5" s="117" t="s">
         <v>532</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="119" t="s">
+      <c r="A6" s="120" t="s">
         <v>533</v>
       </c>
-      <c r="B6" s="120" t="n">
+      <c r="B6" s="121" t="n">
         <v>180</v>
       </c>
-      <c r="C6" s="119" t="s">
+      <c r="C6" s="120" t="s">
         <v>534</v>
       </c>
-      <c r="D6" s="121"/>
-      <c r="E6" s="121"/>
-      <c r="F6" s="121"/>
-      <c r="G6" s="121"/>
-      <c r="H6" s="121"/>
-      <c r="I6" s="120" t="n">
+      <c r="D6" s="122"/>
+      <c r="E6" s="122"/>
+      <c r="F6" s="122"/>
+      <c r="G6" s="122"/>
+      <c r="H6" s="122"/>
+      <c r="I6" s="121" t="n">
         <v>280</v>
       </c>
-      <c r="J6" s="120" t="n">
+      <c r="J6" s="121" t="n">
         <v>330</v>
       </c>
-      <c r="K6" s="121"/>
-      <c r="L6" s="121"/>
-      <c r="M6" s="121"/>
-      <c r="N6" s="119"/>
+      <c r="K6" s="122"/>
+      <c r="L6" s="122"/>
+      <c r="M6" s="122"/>
+      <c r="N6" s="120"/>
     </row>
     <row r="7" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="117" t="s">
+      <c r="A7" s="118" t="s">
         <v>533</v>
       </c>
-      <c r="B7" s="122" t="n">
+      <c r="B7" s="123" t="n">
         <v>365</v>
       </c>
-      <c r="C7" s="117" t="s">
+      <c r="C7" s="118" t="s">
         <v>535</v>
       </c>
-      <c r="D7" s="123"/>
-      <c r="E7" s="123"/>
-      <c r="F7" s="123"/>
-      <c r="G7" s="123"/>
-      <c r="H7" s="123"/>
-      <c r="I7" s="122" t="n">
+      <c r="D7" s="124"/>
+      <c r="E7" s="124"/>
+      <c r="F7" s="124"/>
+      <c r="G7" s="124"/>
+      <c r="H7" s="124"/>
+      <c r="I7" s="123" t="n">
         <v>180</v>
       </c>
-      <c r="J7" s="122" t="n">
+      <c r="J7" s="123" t="n">
         <v>210</v>
       </c>
-      <c r="K7" s="123"/>
-      <c r="L7" s="123"/>
-      <c r="M7" s="123"/>
-      <c r="N7" s="117"/>
+      <c r="K7" s="124"/>
+      <c r="L7" s="124"/>
+      <c r="M7" s="124"/>
+      <c r="N7" s="118"/>
     </row>
     <row r="8" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="124" t="s">
+      <c r="A8" s="125" t="s">
         <v>533</v>
       </c>
-      <c r="B8" s="125" t="n">
+      <c r="B8" s="126" t="n">
         <v>1460</v>
       </c>
-      <c r="C8" s="124" t="s">
+      <c r="C8" s="125" t="s">
         <v>536</v>
       </c>
-      <c r="D8" s="126"/>
-      <c r="E8" s="126"/>
-      <c r="F8" s="126"/>
-      <c r="G8" s="126"/>
-      <c r="H8" s="126"/>
-      <c r="I8" s="125" t="n">
+      <c r="D8" s="127"/>
+      <c r="E8" s="127"/>
+      <c r="F8" s="127"/>
+      <c r="G8" s="127"/>
+      <c r="H8" s="127"/>
+      <c r="I8" s="126" t="n">
         <v>75</v>
       </c>
-      <c r="J8" s="125" t="n">
+      <c r="J8" s="126" t="n">
         <v>90</v>
       </c>
-      <c r="K8" s="126"/>
-      <c r="L8" s="126"/>
-      <c r="M8" s="126"/>
-      <c r="N8" s="124"/>
+      <c r="K8" s="127"/>
+      <c r="L8" s="127"/>
+      <c r="M8" s="127"/>
+      <c r="N8" s="125"/>
     </row>
     <row r="9" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="117" t="s">
+      <c r="A9" s="118" t="s">
         <v>537</v>
       </c>
-      <c r="B9" s="122" t="n">
+      <c r="B9" s="123" t="n">
         <v>180</v>
       </c>
-      <c r="C9" s="117" t="s">
+      <c r="C9" s="118" t="s">
         <v>534</v>
       </c>
-      <c r="D9" s="123"/>
-      <c r="E9" s="123"/>
-      <c r="F9" s="123"/>
-      <c r="G9" s="123"/>
-      <c r="H9" s="123"/>
-      <c r="I9" s="122" t="n">
+      <c r="D9" s="124"/>
+      <c r="E9" s="124"/>
+      <c r="F9" s="124"/>
+      <c r="G9" s="124"/>
+      <c r="H9" s="124"/>
+      <c r="I9" s="123" t="n">
         <v>280</v>
       </c>
-      <c r="J9" s="122" t="n">
+      <c r="J9" s="123" t="n">
         <v>330</v>
       </c>
-      <c r="K9" s="123"/>
-      <c r="L9" s="123"/>
-      <c r="M9" s="123"/>
-      <c r="N9" s="117"/>
+      <c r="K9" s="124"/>
+      <c r="L9" s="124"/>
+      <c r="M9" s="124"/>
+      <c r="N9" s="118"/>
     </row>
     <row r="10" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="124" t="s">
+      <c r="A10" s="125" t="s">
         <v>537</v>
       </c>
-      <c r="B10" s="125" t="n">
+      <c r="B10" s="126" t="n">
         <v>365</v>
       </c>
-      <c r="C10" s="124" t="s">
+      <c r="C10" s="125" t="s">
         <v>535</v>
       </c>
-      <c r="D10" s="126"/>
-      <c r="E10" s="126"/>
-      <c r="F10" s="126"/>
-      <c r="G10" s="126"/>
-      <c r="H10" s="126"/>
-      <c r="I10" s="125" t="n">
+      <c r="D10" s="127"/>
+      <c r="E10" s="127"/>
+      <c r="F10" s="127"/>
+      <c r="G10" s="127"/>
+      <c r="H10" s="127"/>
+      <c r="I10" s="126" t="n">
         <v>180</v>
       </c>
-      <c r="J10" s="125" t="n">
+      <c r="J10" s="126" t="n">
         <v>210</v>
       </c>
-      <c r="K10" s="126"/>
-      <c r="L10" s="126"/>
-      <c r="M10" s="126"/>
-      <c r="N10" s="124"/>
+      <c r="K10" s="127"/>
+      <c r="L10" s="127"/>
+      <c r="M10" s="127"/>
+      <c r="N10" s="125"/>
     </row>
     <row r="11" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A11" s="117" t="s">
+      <c r="A11" s="118" t="s">
         <v>537</v>
       </c>
-      <c r="B11" s="122" t="n">
+      <c r="B11" s="123" t="n">
         <v>1460</v>
       </c>
-      <c r="C11" s="117" t="s">
+      <c r="C11" s="118" t="s">
         <v>536</v>
       </c>
-      <c r="D11" s="123"/>
-      <c r="E11" s="123"/>
-      <c r="F11" s="123"/>
-      <c r="G11" s="123"/>
-      <c r="H11" s="123"/>
-      <c r="I11" s="122" t="n">
+      <c r="D11" s="124"/>
+      <c r="E11" s="124"/>
+      <c r="F11" s="124"/>
+      <c r="G11" s="124"/>
+      <c r="H11" s="124"/>
+      <c r="I11" s="123" t="n">
         <v>75</v>
       </c>
-      <c r="J11" s="122" t="n">
+      <c r="J11" s="123" t="n">
         <v>90</v>
       </c>
-      <c r="K11" s="123"/>
-      <c r="L11" s="123"/>
-      <c r="M11" s="123"/>
-      <c r="N11" s="117"/>
+      <c r="K11" s="124"/>
+      <c r="L11" s="124"/>
+      <c r="M11" s="124"/>
+      <c r="N11" s="118"/>
     </row>
     <row r="12" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A12" s="124" t="s">
+      <c r="A12" s="125" t="s">
         <v>533</v>
       </c>
-      <c r="B12" s="125" t="n">
+      <c r="B12" s="126" t="n">
         <v>65535</v>
       </c>
-      <c r="C12" s="124" t="s">
+      <c r="C12" s="125" t="s">
         <v>538</v>
       </c>
-      <c r="D12" s="126"/>
-      <c r="E12" s="126"/>
-      <c r="F12" s="126"/>
-      <c r="G12" s="126"/>
-      <c r="H12" s="126"/>
-      <c r="I12" s="125" t="n">
+      <c r="D12" s="127"/>
+      <c r="E12" s="127"/>
+      <c r="F12" s="127"/>
+      <c r="G12" s="127"/>
+      <c r="H12" s="127"/>
+      <c r="I12" s="126" t="n">
         <v>50</v>
       </c>
-      <c r="J12" s="125" t="n">
+      <c r="J12" s="126" t="n">
         <v>65</v>
       </c>
-      <c r="K12" s="126"/>
-      <c r="L12" s="126"/>
-      <c r="M12" s="126"/>
-      <c r="N12" s="124"/>
+      <c r="K12" s="127"/>
+      <c r="L12" s="127"/>
+      <c r="M12" s="127"/>
+      <c r="N12" s="125"/>
     </row>
     <row r="13" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A13" s="117" t="s">
+      <c r="A13" s="118" t="s">
         <v>537</v>
       </c>
-      <c r="B13" s="122" t="n">
+      <c r="B13" s="123" t="n">
         <v>65535</v>
       </c>
-      <c r="C13" s="117" t="s">
+      <c r="C13" s="118" t="s">
         <v>538</v>
       </c>
-      <c r="D13" s="123"/>
-      <c r="E13" s="123"/>
-      <c r="F13" s="123"/>
-      <c r="G13" s="123"/>
-      <c r="H13" s="123"/>
-      <c r="I13" s="122" t="n">
+      <c r="D13" s="124"/>
+      <c r="E13" s="124"/>
+      <c r="F13" s="124"/>
+      <c r="G13" s="124"/>
+      <c r="H13" s="124"/>
+      <c r="I13" s="123" t="n">
         <v>50</v>
       </c>
-      <c r="J13" s="122" t="n">
+      <c r="J13" s="123" t="n">
         <v>65</v>
       </c>
-      <c r="K13" s="123"/>
-      <c r="L13" s="123"/>
-      <c r="M13" s="123"/>
-      <c r="N13" s="117"/>
+      <c r="K13" s="124"/>
+      <c r="L13" s="124"/>
+      <c r="M13" s="124"/>
+      <c r="N13" s="118"/>
     </row>
     <row r="14" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A14" s="124" t="s">
+      <c r="A14" s="125" t="s">
         <v>539</v>
       </c>
-      <c r="B14" s="125" t="n">
+      <c r="B14" s="126" t="n">
         <v>180</v>
       </c>
-      <c r="C14" s="124" t="s">
+      <c r="C14" s="125" t="s">
         <v>534</v>
       </c>
-      <c r="D14" s="126"/>
-      <c r="E14" s="126"/>
-      <c r="F14" s="126"/>
-      <c r="G14" s="126"/>
-      <c r="H14" s="126"/>
-      <c r="I14" s="125" t="n">
+      <c r="D14" s="127"/>
+      <c r="E14" s="127"/>
+      <c r="F14" s="127"/>
+      <c r="G14" s="127"/>
+      <c r="H14" s="127"/>
+      <c r="I14" s="126" t="n">
         <v>280</v>
       </c>
-      <c r="J14" s="125" t="n">
+      <c r="J14" s="126" t="n">
         <v>330</v>
       </c>
-      <c r="K14" s="126"/>
-      <c r="L14" s="126"/>
-      <c r="M14" s="126"/>
-      <c r="N14" s="124"/>
+      <c r="K14" s="127"/>
+      <c r="L14" s="127"/>
+      <c r="M14" s="127"/>
+      <c r="N14" s="125"/>
     </row>
     <row r="15" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A15" s="117" t="s">
+      <c r="A15" s="118" t="s">
         <v>539</v>
       </c>
-      <c r="B15" s="122" t="n">
+      <c r="B15" s="123" t="n">
         <v>365</v>
       </c>
-      <c r="C15" s="117" t="s">
+      <c r="C15" s="118" t="s">
         <v>535</v>
       </c>
-      <c r="D15" s="123"/>
-      <c r="E15" s="123"/>
-      <c r="F15" s="123"/>
-      <c r="G15" s="123"/>
-      <c r="H15" s="123"/>
-      <c r="I15" s="122" t="n">
+      <c r="D15" s="124"/>
+      <c r="E15" s="124"/>
+      <c r="F15" s="124"/>
+      <c r="G15" s="124"/>
+      <c r="H15" s="124"/>
+      <c r="I15" s="123" t="n">
         <v>180</v>
       </c>
-      <c r="J15" s="122" t="n">
+      <c r="J15" s="123" t="n">
         <v>210</v>
       </c>
-      <c r="K15" s="123"/>
-      <c r="L15" s="123"/>
-      <c r="M15" s="123"/>
-      <c r="N15" s="117"/>
+      <c r="K15" s="124"/>
+      <c r="L15" s="124"/>
+      <c r="M15" s="124"/>
+      <c r="N15" s="118"/>
     </row>
     <row r="16" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A16" s="124" t="s">
+      <c r="A16" s="125" t="s">
         <v>539</v>
       </c>
-      <c r="B16" s="125" t="n">
+      <c r="B16" s="126" t="n">
         <v>1460</v>
       </c>
-      <c r="C16" s="124" t="s">
+      <c r="C16" s="125" t="s">
         <v>536</v>
       </c>
-      <c r="D16" s="126"/>
-      <c r="E16" s="126"/>
-      <c r="F16" s="126"/>
-      <c r="G16" s="126"/>
-      <c r="H16" s="126"/>
-      <c r="I16" s="125" t="n">
+      <c r="D16" s="127"/>
+      <c r="E16" s="127"/>
+      <c r="F16" s="127"/>
+      <c r="G16" s="127"/>
+      <c r="H16" s="127"/>
+      <c r="I16" s="126" t="n">
         <v>75</v>
       </c>
-      <c r="J16" s="125" t="n">
+      <c r="J16" s="126" t="n">
         <v>90</v>
       </c>
-      <c r="K16" s="126"/>
-      <c r="L16" s="126"/>
-      <c r="M16" s="126"/>
-      <c r="N16" s="124"/>
+      <c r="K16" s="127"/>
+      <c r="L16" s="127"/>
+      <c r="M16" s="127"/>
+      <c r="N16" s="125"/>
     </row>
     <row r="17" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A17" s="117" t="s">
+      <c r="A17" s="118" t="s">
         <v>537</v>
       </c>
-      <c r="B17" s="122" t="n">
+      <c r="B17" s="123" t="n">
         <v>4380</v>
       </c>
-      <c r="C17" s="117" t="s">
+      <c r="C17" s="118" t="s">
         <v>538</v>
       </c>
-      <c r="D17" s="123"/>
-      <c r="E17" s="123"/>
-      <c r="F17" s="123"/>
-      <c r="G17" s="123"/>
-      <c r="H17" s="123"/>
-      <c r="I17" s="122" t="n">
+      <c r="D17" s="124"/>
+      <c r="E17" s="124"/>
+      <c r="F17" s="124"/>
+      <c r="G17" s="124"/>
+      <c r="H17" s="124"/>
+      <c r="I17" s="123" t="n">
         <v>50</v>
       </c>
-      <c r="J17" s="123"/>
-      <c r="K17" s="123"/>
-      <c r="L17" s="123"/>
-      <c r="M17" s="123"/>
-      <c r="N17" s="117"/>
+      <c r="J17" s="124"/>
+      <c r="K17" s="124"/>
+      <c r="L17" s="124"/>
+      <c r="M17" s="124"/>
+      <c r="N17" s="118"/>
     </row>
     <row r="18" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A18" s="124" t="s">
+      <c r="A18" s="125" t="s">
         <v>533</v>
       </c>
-      <c r="B18" s="125" t="n">
+      <c r="B18" s="126" t="n">
         <v>4380</v>
       </c>
-      <c r="C18" s="124" t="s">
+      <c r="C18" s="125" t="s">
         <v>538</v>
       </c>
-      <c r="D18" s="126"/>
-      <c r="E18" s="126"/>
-      <c r="F18" s="126"/>
-      <c r="G18" s="126"/>
-      <c r="H18" s="126"/>
-      <c r="I18" s="125" t="n">
+      <c r="D18" s="127"/>
+      <c r="E18" s="127"/>
+      <c r="F18" s="127"/>
+      <c r="G18" s="127"/>
+      <c r="H18" s="127"/>
+      <c r="I18" s="126" t="n">
         <v>50</v>
       </c>
-      <c r="J18" s="126"/>
-      <c r="K18" s="126"/>
-      <c r="L18" s="126"/>
-      <c r="M18" s="126"/>
-      <c r="N18" s="124"/>
+      <c r="J18" s="127"/>
+      <c r="K18" s="127"/>
+      <c r="L18" s="127"/>
+      <c r="M18" s="127"/>
+      <c r="N18" s="125"/>
     </row>
     <row r="19" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A19" s="117" t="s">
+      <c r="A19" s="118" t="s">
         <v>539</v>
       </c>
-      <c r="B19" s="122" t="n">
+      <c r="B19" s="123" t="n">
         <v>4380</v>
       </c>
-      <c r="C19" s="117" t="s">
+      <c r="C19" s="118" t="s">
         <v>538</v>
       </c>
-      <c r="D19" s="123"/>
-      <c r="E19" s="123"/>
-      <c r="F19" s="123"/>
-      <c r="G19" s="123"/>
-      <c r="H19" s="123"/>
-      <c r="I19" s="122" t="n">
+      <c r="D19" s="124"/>
+      <c r="E19" s="124"/>
+      <c r="F19" s="124"/>
+      <c r="G19" s="124"/>
+      <c r="H19" s="124"/>
+      <c r="I19" s="123" t="n">
         <v>50</v>
       </c>
-      <c r="J19" s="123"/>
-      <c r="K19" s="123"/>
-      <c r="L19" s="123"/>
-      <c r="M19" s="123"/>
-      <c r="N19" s="117"/>
+      <c r="J19" s="124"/>
+      <c r="K19" s="124"/>
+      <c r="L19" s="124"/>
+      <c r="M19" s="124"/>
+      <c r="N19" s="118"/>
     </row>
     <row r="22" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">

</xml_diff>